<commit_message>
add new files & save changes
</commit_message>
<xml_diff>
--- a/product.docs/算法匹配.xlsx
+++ b/product.docs/算法匹配.xlsx
@@ -9,7 +9,6 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -877,10 +876,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -1064,7 +1063,7 @@
     <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1073,11 +1072,11 @@
     <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1088,15 +1087,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1530,11 +1520,11 @@
         </a:custGeom>
         <a:gradFill rotWithShape="0">
           <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="BBD5F0"/>
+            </a:gs>
             <a:gs pos="100000">
               <a:srgbClr val="9CBEE0"/>
-            </a:gs>
-            <a:gs pos="0">
-              <a:srgbClr val="BBD5F0"/>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
@@ -1566,2175 +1556,2175 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="7" customWidth="1"/>
-    <col min="2" max="2" width="21.375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="18.625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="23.125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="20.875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="21.125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="13" style="7" customWidth="1"/>
-    <col min="8" max="9" width="19.75" style="7" customWidth="1"/>
-    <col min="10" max="10" width="24.75" style="7" customWidth="1"/>
-    <col min="11" max="11" width="14.625" style="7" customWidth="1"/>
-    <col min="12" max="12" width="19.75" style="7" customWidth="1"/>
-    <col min="13" max="256" width="9" style="7"/>
-    <col min="257" max="257" width="11.5" style="7" customWidth="1"/>
-    <col min="258" max="258" width="21.375" style="7" customWidth="1"/>
-    <col min="259" max="259" width="18.625" style="7" customWidth="1"/>
-    <col min="260" max="260" width="23.125" style="7" customWidth="1"/>
-    <col min="261" max="261" width="20.875" style="7" customWidth="1"/>
-    <col min="262" max="262" width="21.125" style="7" customWidth="1"/>
-    <col min="263" max="263" width="13" style="7" customWidth="1"/>
-    <col min="264" max="265" width="19.75" style="7" customWidth="1"/>
-    <col min="266" max="266" width="24.75" style="7" customWidth="1"/>
-    <col min="267" max="267" width="14.625" style="7" customWidth="1"/>
-    <col min="268" max="268" width="19.75" style="7" customWidth="1"/>
-    <col min="269" max="512" width="9" style="7"/>
-    <col min="513" max="513" width="11.5" style="7" customWidth="1"/>
-    <col min="514" max="514" width="21.375" style="7" customWidth="1"/>
-    <col min="515" max="515" width="18.625" style="7" customWidth="1"/>
-    <col min="516" max="516" width="23.125" style="7" customWidth="1"/>
-    <col min="517" max="517" width="20.875" style="7" customWidth="1"/>
-    <col min="518" max="518" width="21.125" style="7" customWidth="1"/>
-    <col min="519" max="519" width="13" style="7" customWidth="1"/>
-    <col min="520" max="521" width="19.75" style="7" customWidth="1"/>
-    <col min="522" max="522" width="24.75" style="7" customWidth="1"/>
-    <col min="523" max="523" width="14.625" style="7" customWidth="1"/>
-    <col min="524" max="524" width="19.75" style="7" customWidth="1"/>
-    <col min="525" max="768" width="9" style="7"/>
-    <col min="769" max="769" width="11.5" style="7" customWidth="1"/>
-    <col min="770" max="770" width="21.375" style="7" customWidth="1"/>
-    <col min="771" max="771" width="18.625" style="7" customWidth="1"/>
-    <col min="772" max="772" width="23.125" style="7" customWidth="1"/>
-    <col min="773" max="773" width="20.875" style="7" customWidth="1"/>
-    <col min="774" max="774" width="21.125" style="7" customWidth="1"/>
-    <col min="775" max="775" width="13" style="7" customWidth="1"/>
-    <col min="776" max="777" width="19.75" style="7" customWidth="1"/>
-    <col min="778" max="778" width="24.75" style="7" customWidth="1"/>
-    <col min="779" max="779" width="14.625" style="7" customWidth="1"/>
-    <col min="780" max="780" width="19.75" style="7" customWidth="1"/>
-    <col min="781" max="1024" width="9" style="7"/>
-    <col min="1025" max="1025" width="11.5" style="7" customWidth="1"/>
-    <col min="1026" max="1026" width="21.375" style="7" customWidth="1"/>
-    <col min="1027" max="1027" width="18.625" style="7" customWidth="1"/>
-    <col min="1028" max="1028" width="23.125" style="7" customWidth="1"/>
-    <col min="1029" max="1029" width="20.875" style="7" customWidth="1"/>
-    <col min="1030" max="1030" width="21.125" style="7" customWidth="1"/>
-    <col min="1031" max="1031" width="13" style="7" customWidth="1"/>
-    <col min="1032" max="1033" width="19.75" style="7" customWidth="1"/>
-    <col min="1034" max="1034" width="24.75" style="7" customWidth="1"/>
-    <col min="1035" max="1035" width="14.625" style="7" customWidth="1"/>
-    <col min="1036" max="1036" width="19.75" style="7" customWidth="1"/>
-    <col min="1037" max="1280" width="9" style="7"/>
-    <col min="1281" max="1281" width="11.5" style="7" customWidth="1"/>
-    <col min="1282" max="1282" width="21.375" style="7" customWidth="1"/>
-    <col min="1283" max="1283" width="18.625" style="7" customWidth="1"/>
-    <col min="1284" max="1284" width="23.125" style="7" customWidth="1"/>
-    <col min="1285" max="1285" width="20.875" style="7" customWidth="1"/>
-    <col min="1286" max="1286" width="21.125" style="7" customWidth="1"/>
-    <col min="1287" max="1287" width="13" style="7" customWidth="1"/>
-    <col min="1288" max="1289" width="19.75" style="7" customWidth="1"/>
-    <col min="1290" max="1290" width="24.75" style="7" customWidth="1"/>
-    <col min="1291" max="1291" width="14.625" style="7" customWidth="1"/>
-    <col min="1292" max="1292" width="19.75" style="7" customWidth="1"/>
-    <col min="1293" max="1536" width="9" style="7"/>
-    <col min="1537" max="1537" width="11.5" style="7" customWidth="1"/>
-    <col min="1538" max="1538" width="21.375" style="7" customWidth="1"/>
-    <col min="1539" max="1539" width="18.625" style="7" customWidth="1"/>
-    <col min="1540" max="1540" width="23.125" style="7" customWidth="1"/>
-    <col min="1541" max="1541" width="20.875" style="7" customWidth="1"/>
-    <col min="1542" max="1542" width="21.125" style="7" customWidth="1"/>
-    <col min="1543" max="1543" width="13" style="7" customWidth="1"/>
-    <col min="1544" max="1545" width="19.75" style="7" customWidth="1"/>
-    <col min="1546" max="1546" width="24.75" style="7" customWidth="1"/>
-    <col min="1547" max="1547" width="14.625" style="7" customWidth="1"/>
-    <col min="1548" max="1548" width="19.75" style="7" customWidth="1"/>
-    <col min="1549" max="1792" width="9" style="7"/>
-    <col min="1793" max="1793" width="11.5" style="7" customWidth="1"/>
-    <col min="1794" max="1794" width="21.375" style="7" customWidth="1"/>
-    <col min="1795" max="1795" width="18.625" style="7" customWidth="1"/>
-    <col min="1796" max="1796" width="23.125" style="7" customWidth="1"/>
-    <col min="1797" max="1797" width="20.875" style="7" customWidth="1"/>
-    <col min="1798" max="1798" width="21.125" style="7" customWidth="1"/>
-    <col min="1799" max="1799" width="13" style="7" customWidth="1"/>
-    <col min="1800" max="1801" width="19.75" style="7" customWidth="1"/>
-    <col min="1802" max="1802" width="24.75" style="7" customWidth="1"/>
-    <col min="1803" max="1803" width="14.625" style="7" customWidth="1"/>
-    <col min="1804" max="1804" width="19.75" style="7" customWidth="1"/>
-    <col min="1805" max="2048" width="9" style="7"/>
-    <col min="2049" max="2049" width="11.5" style="7" customWidth="1"/>
-    <col min="2050" max="2050" width="21.375" style="7" customWidth="1"/>
-    <col min="2051" max="2051" width="18.625" style="7" customWidth="1"/>
-    <col min="2052" max="2052" width="23.125" style="7" customWidth="1"/>
-    <col min="2053" max="2053" width="20.875" style="7" customWidth="1"/>
-    <col min="2054" max="2054" width="21.125" style="7" customWidth="1"/>
-    <col min="2055" max="2055" width="13" style="7" customWidth="1"/>
-    <col min="2056" max="2057" width="19.75" style="7" customWidth="1"/>
-    <col min="2058" max="2058" width="24.75" style="7" customWidth="1"/>
-    <col min="2059" max="2059" width="14.625" style="7" customWidth="1"/>
-    <col min="2060" max="2060" width="19.75" style="7" customWidth="1"/>
-    <col min="2061" max="2304" width="9" style="7"/>
-    <col min="2305" max="2305" width="11.5" style="7" customWidth="1"/>
-    <col min="2306" max="2306" width="21.375" style="7" customWidth="1"/>
-    <col min="2307" max="2307" width="18.625" style="7" customWidth="1"/>
-    <col min="2308" max="2308" width="23.125" style="7" customWidth="1"/>
-    <col min="2309" max="2309" width="20.875" style="7" customWidth="1"/>
-    <col min="2310" max="2310" width="21.125" style="7" customWidth="1"/>
-    <col min="2311" max="2311" width="13" style="7" customWidth="1"/>
-    <col min="2312" max="2313" width="19.75" style="7" customWidth="1"/>
-    <col min="2314" max="2314" width="24.75" style="7" customWidth="1"/>
-    <col min="2315" max="2315" width="14.625" style="7" customWidth="1"/>
-    <col min="2316" max="2316" width="19.75" style="7" customWidth="1"/>
-    <col min="2317" max="2560" width="9" style="7"/>
-    <col min="2561" max="2561" width="11.5" style="7" customWidth="1"/>
-    <col min="2562" max="2562" width="21.375" style="7" customWidth="1"/>
-    <col min="2563" max="2563" width="18.625" style="7" customWidth="1"/>
-    <col min="2564" max="2564" width="23.125" style="7" customWidth="1"/>
-    <col min="2565" max="2565" width="20.875" style="7" customWidth="1"/>
-    <col min="2566" max="2566" width="21.125" style="7" customWidth="1"/>
-    <col min="2567" max="2567" width="13" style="7" customWidth="1"/>
-    <col min="2568" max="2569" width="19.75" style="7" customWidth="1"/>
-    <col min="2570" max="2570" width="24.75" style="7" customWidth="1"/>
-    <col min="2571" max="2571" width="14.625" style="7" customWidth="1"/>
-    <col min="2572" max="2572" width="19.75" style="7" customWidth="1"/>
-    <col min="2573" max="2816" width="9" style="7"/>
-    <col min="2817" max="2817" width="11.5" style="7" customWidth="1"/>
-    <col min="2818" max="2818" width="21.375" style="7" customWidth="1"/>
-    <col min="2819" max="2819" width="18.625" style="7" customWidth="1"/>
-    <col min="2820" max="2820" width="23.125" style="7" customWidth="1"/>
-    <col min="2821" max="2821" width="20.875" style="7" customWidth="1"/>
-    <col min="2822" max="2822" width="21.125" style="7" customWidth="1"/>
-    <col min="2823" max="2823" width="13" style="7" customWidth="1"/>
-    <col min="2824" max="2825" width="19.75" style="7" customWidth="1"/>
-    <col min="2826" max="2826" width="24.75" style="7" customWidth="1"/>
-    <col min="2827" max="2827" width="14.625" style="7" customWidth="1"/>
-    <col min="2828" max="2828" width="19.75" style="7" customWidth="1"/>
-    <col min="2829" max="3072" width="9" style="7"/>
-    <col min="3073" max="3073" width="11.5" style="7" customWidth="1"/>
-    <col min="3074" max="3074" width="21.375" style="7" customWidth="1"/>
-    <col min="3075" max="3075" width="18.625" style="7" customWidth="1"/>
-    <col min="3076" max="3076" width="23.125" style="7" customWidth="1"/>
-    <col min="3077" max="3077" width="20.875" style="7" customWidth="1"/>
-    <col min="3078" max="3078" width="21.125" style="7" customWidth="1"/>
-    <col min="3079" max="3079" width="13" style="7" customWidth="1"/>
-    <col min="3080" max="3081" width="19.75" style="7" customWidth="1"/>
-    <col min="3082" max="3082" width="24.75" style="7" customWidth="1"/>
-    <col min="3083" max="3083" width="14.625" style="7" customWidth="1"/>
-    <col min="3084" max="3084" width="19.75" style="7" customWidth="1"/>
-    <col min="3085" max="3328" width="9" style="7"/>
-    <col min="3329" max="3329" width="11.5" style="7" customWidth="1"/>
-    <col min="3330" max="3330" width="21.375" style="7" customWidth="1"/>
-    <col min="3331" max="3331" width="18.625" style="7" customWidth="1"/>
-    <col min="3332" max="3332" width="23.125" style="7" customWidth="1"/>
-    <col min="3333" max="3333" width="20.875" style="7" customWidth="1"/>
-    <col min="3334" max="3334" width="21.125" style="7" customWidth="1"/>
-    <col min="3335" max="3335" width="13" style="7" customWidth="1"/>
-    <col min="3336" max="3337" width="19.75" style="7" customWidth="1"/>
-    <col min="3338" max="3338" width="24.75" style="7" customWidth="1"/>
-    <col min="3339" max="3339" width="14.625" style="7" customWidth="1"/>
-    <col min="3340" max="3340" width="19.75" style="7" customWidth="1"/>
-    <col min="3341" max="3584" width="9" style="7"/>
-    <col min="3585" max="3585" width="11.5" style="7" customWidth="1"/>
-    <col min="3586" max="3586" width="21.375" style="7" customWidth="1"/>
-    <col min="3587" max="3587" width="18.625" style="7" customWidth="1"/>
-    <col min="3588" max="3588" width="23.125" style="7" customWidth="1"/>
-    <col min="3589" max="3589" width="20.875" style="7" customWidth="1"/>
-    <col min="3590" max="3590" width="21.125" style="7" customWidth="1"/>
-    <col min="3591" max="3591" width="13" style="7" customWidth="1"/>
-    <col min="3592" max="3593" width="19.75" style="7" customWidth="1"/>
-    <col min="3594" max="3594" width="24.75" style="7" customWidth="1"/>
-    <col min="3595" max="3595" width="14.625" style="7" customWidth="1"/>
-    <col min="3596" max="3596" width="19.75" style="7" customWidth="1"/>
-    <col min="3597" max="3840" width="9" style="7"/>
-    <col min="3841" max="3841" width="11.5" style="7" customWidth="1"/>
-    <col min="3842" max="3842" width="21.375" style="7" customWidth="1"/>
-    <col min="3843" max="3843" width="18.625" style="7" customWidth="1"/>
-    <col min="3844" max="3844" width="23.125" style="7" customWidth="1"/>
-    <col min="3845" max="3845" width="20.875" style="7" customWidth="1"/>
-    <col min="3846" max="3846" width="21.125" style="7" customWidth="1"/>
-    <col min="3847" max="3847" width="13" style="7" customWidth="1"/>
-    <col min="3848" max="3849" width="19.75" style="7" customWidth="1"/>
-    <col min="3850" max="3850" width="24.75" style="7" customWidth="1"/>
-    <col min="3851" max="3851" width="14.625" style="7" customWidth="1"/>
-    <col min="3852" max="3852" width="19.75" style="7" customWidth="1"/>
-    <col min="3853" max="4096" width="9" style="7"/>
-    <col min="4097" max="4097" width="11.5" style="7" customWidth="1"/>
-    <col min="4098" max="4098" width="21.375" style="7" customWidth="1"/>
-    <col min="4099" max="4099" width="18.625" style="7" customWidth="1"/>
-    <col min="4100" max="4100" width="23.125" style="7" customWidth="1"/>
-    <col min="4101" max="4101" width="20.875" style="7" customWidth="1"/>
-    <col min="4102" max="4102" width="21.125" style="7" customWidth="1"/>
-    <col min="4103" max="4103" width="13" style="7" customWidth="1"/>
-    <col min="4104" max="4105" width="19.75" style="7" customWidth="1"/>
-    <col min="4106" max="4106" width="24.75" style="7" customWidth="1"/>
-    <col min="4107" max="4107" width="14.625" style="7" customWidth="1"/>
-    <col min="4108" max="4108" width="19.75" style="7" customWidth="1"/>
-    <col min="4109" max="4352" width="9" style="7"/>
-    <col min="4353" max="4353" width="11.5" style="7" customWidth="1"/>
-    <col min="4354" max="4354" width="21.375" style="7" customWidth="1"/>
-    <col min="4355" max="4355" width="18.625" style="7" customWidth="1"/>
-    <col min="4356" max="4356" width="23.125" style="7" customWidth="1"/>
-    <col min="4357" max="4357" width="20.875" style="7" customWidth="1"/>
-    <col min="4358" max="4358" width="21.125" style="7" customWidth="1"/>
-    <col min="4359" max="4359" width="13" style="7" customWidth="1"/>
-    <col min="4360" max="4361" width="19.75" style="7" customWidth="1"/>
-    <col min="4362" max="4362" width="24.75" style="7" customWidth="1"/>
-    <col min="4363" max="4363" width="14.625" style="7" customWidth="1"/>
-    <col min="4364" max="4364" width="19.75" style="7" customWidth="1"/>
-    <col min="4365" max="4608" width="9" style="7"/>
-    <col min="4609" max="4609" width="11.5" style="7" customWidth="1"/>
-    <col min="4610" max="4610" width="21.375" style="7" customWidth="1"/>
-    <col min="4611" max="4611" width="18.625" style="7" customWidth="1"/>
-    <col min="4612" max="4612" width="23.125" style="7" customWidth="1"/>
-    <col min="4613" max="4613" width="20.875" style="7" customWidth="1"/>
-    <col min="4614" max="4614" width="21.125" style="7" customWidth="1"/>
-    <col min="4615" max="4615" width="13" style="7" customWidth="1"/>
-    <col min="4616" max="4617" width="19.75" style="7" customWidth="1"/>
-    <col min="4618" max="4618" width="24.75" style="7" customWidth="1"/>
-    <col min="4619" max="4619" width="14.625" style="7" customWidth="1"/>
-    <col min="4620" max="4620" width="19.75" style="7" customWidth="1"/>
-    <col min="4621" max="4864" width="9" style="7"/>
-    <col min="4865" max="4865" width="11.5" style="7" customWidth="1"/>
-    <col min="4866" max="4866" width="21.375" style="7" customWidth="1"/>
-    <col min="4867" max="4867" width="18.625" style="7" customWidth="1"/>
-    <col min="4868" max="4868" width="23.125" style="7" customWidth="1"/>
-    <col min="4869" max="4869" width="20.875" style="7" customWidth="1"/>
-    <col min="4870" max="4870" width="21.125" style="7" customWidth="1"/>
-    <col min="4871" max="4871" width="13" style="7" customWidth="1"/>
-    <col min="4872" max="4873" width="19.75" style="7" customWidth="1"/>
-    <col min="4874" max="4874" width="24.75" style="7" customWidth="1"/>
-    <col min="4875" max="4875" width="14.625" style="7" customWidth="1"/>
-    <col min="4876" max="4876" width="19.75" style="7" customWidth="1"/>
-    <col min="4877" max="5120" width="9" style="7"/>
-    <col min="5121" max="5121" width="11.5" style="7" customWidth="1"/>
-    <col min="5122" max="5122" width="21.375" style="7" customWidth="1"/>
-    <col min="5123" max="5123" width="18.625" style="7" customWidth="1"/>
-    <col min="5124" max="5124" width="23.125" style="7" customWidth="1"/>
-    <col min="5125" max="5125" width="20.875" style="7" customWidth="1"/>
-    <col min="5126" max="5126" width="21.125" style="7" customWidth="1"/>
-    <col min="5127" max="5127" width="13" style="7" customWidth="1"/>
-    <col min="5128" max="5129" width="19.75" style="7" customWidth="1"/>
-    <col min="5130" max="5130" width="24.75" style="7" customWidth="1"/>
-    <col min="5131" max="5131" width="14.625" style="7" customWidth="1"/>
-    <col min="5132" max="5132" width="19.75" style="7" customWidth="1"/>
-    <col min="5133" max="5376" width="9" style="7"/>
-    <col min="5377" max="5377" width="11.5" style="7" customWidth="1"/>
-    <col min="5378" max="5378" width="21.375" style="7" customWidth="1"/>
-    <col min="5379" max="5379" width="18.625" style="7" customWidth="1"/>
-    <col min="5380" max="5380" width="23.125" style="7" customWidth="1"/>
-    <col min="5381" max="5381" width="20.875" style="7" customWidth="1"/>
-    <col min="5382" max="5382" width="21.125" style="7" customWidth="1"/>
-    <col min="5383" max="5383" width="13" style="7" customWidth="1"/>
-    <col min="5384" max="5385" width="19.75" style="7" customWidth="1"/>
-    <col min="5386" max="5386" width="24.75" style="7" customWidth="1"/>
-    <col min="5387" max="5387" width="14.625" style="7" customWidth="1"/>
-    <col min="5388" max="5388" width="19.75" style="7" customWidth="1"/>
-    <col min="5389" max="5632" width="9" style="7"/>
-    <col min="5633" max="5633" width="11.5" style="7" customWidth="1"/>
-    <col min="5634" max="5634" width="21.375" style="7" customWidth="1"/>
-    <col min="5635" max="5635" width="18.625" style="7" customWidth="1"/>
-    <col min="5636" max="5636" width="23.125" style="7" customWidth="1"/>
-    <col min="5637" max="5637" width="20.875" style="7" customWidth="1"/>
-    <col min="5638" max="5638" width="21.125" style="7" customWidth="1"/>
-    <col min="5639" max="5639" width="13" style="7" customWidth="1"/>
-    <col min="5640" max="5641" width="19.75" style="7" customWidth="1"/>
-    <col min="5642" max="5642" width="24.75" style="7" customWidth="1"/>
-    <col min="5643" max="5643" width="14.625" style="7" customWidth="1"/>
-    <col min="5644" max="5644" width="19.75" style="7" customWidth="1"/>
-    <col min="5645" max="5888" width="9" style="7"/>
-    <col min="5889" max="5889" width="11.5" style="7" customWidth="1"/>
-    <col min="5890" max="5890" width="21.375" style="7" customWidth="1"/>
-    <col min="5891" max="5891" width="18.625" style="7" customWidth="1"/>
-    <col min="5892" max="5892" width="23.125" style="7" customWidth="1"/>
-    <col min="5893" max="5893" width="20.875" style="7" customWidth="1"/>
-    <col min="5894" max="5894" width="21.125" style="7" customWidth="1"/>
-    <col min="5895" max="5895" width="13" style="7" customWidth="1"/>
-    <col min="5896" max="5897" width="19.75" style="7" customWidth="1"/>
-    <col min="5898" max="5898" width="24.75" style="7" customWidth="1"/>
-    <col min="5899" max="5899" width="14.625" style="7" customWidth="1"/>
-    <col min="5900" max="5900" width="19.75" style="7" customWidth="1"/>
-    <col min="5901" max="6144" width="9" style="7"/>
-    <col min="6145" max="6145" width="11.5" style="7" customWidth="1"/>
-    <col min="6146" max="6146" width="21.375" style="7" customWidth="1"/>
-    <col min="6147" max="6147" width="18.625" style="7" customWidth="1"/>
-    <col min="6148" max="6148" width="23.125" style="7" customWidth="1"/>
-    <col min="6149" max="6149" width="20.875" style="7" customWidth="1"/>
-    <col min="6150" max="6150" width="21.125" style="7" customWidth="1"/>
-    <col min="6151" max="6151" width="13" style="7" customWidth="1"/>
-    <col min="6152" max="6153" width="19.75" style="7" customWidth="1"/>
-    <col min="6154" max="6154" width="24.75" style="7" customWidth="1"/>
-    <col min="6155" max="6155" width="14.625" style="7" customWidth="1"/>
-    <col min="6156" max="6156" width="19.75" style="7" customWidth="1"/>
-    <col min="6157" max="6400" width="9" style="7"/>
-    <col min="6401" max="6401" width="11.5" style="7" customWidth="1"/>
-    <col min="6402" max="6402" width="21.375" style="7" customWidth="1"/>
-    <col min="6403" max="6403" width="18.625" style="7" customWidth="1"/>
-    <col min="6404" max="6404" width="23.125" style="7" customWidth="1"/>
-    <col min="6405" max="6405" width="20.875" style="7" customWidth="1"/>
-    <col min="6406" max="6406" width="21.125" style="7" customWidth="1"/>
-    <col min="6407" max="6407" width="13" style="7" customWidth="1"/>
-    <col min="6408" max="6409" width="19.75" style="7" customWidth="1"/>
-    <col min="6410" max="6410" width="24.75" style="7" customWidth="1"/>
-    <col min="6411" max="6411" width="14.625" style="7" customWidth="1"/>
-    <col min="6412" max="6412" width="19.75" style="7" customWidth="1"/>
-    <col min="6413" max="6656" width="9" style="7"/>
-    <col min="6657" max="6657" width="11.5" style="7" customWidth="1"/>
-    <col min="6658" max="6658" width="21.375" style="7" customWidth="1"/>
-    <col min="6659" max="6659" width="18.625" style="7" customWidth="1"/>
-    <col min="6660" max="6660" width="23.125" style="7" customWidth="1"/>
-    <col min="6661" max="6661" width="20.875" style="7" customWidth="1"/>
-    <col min="6662" max="6662" width="21.125" style="7" customWidth="1"/>
-    <col min="6663" max="6663" width="13" style="7" customWidth="1"/>
-    <col min="6664" max="6665" width="19.75" style="7" customWidth="1"/>
-    <col min="6666" max="6666" width="24.75" style="7" customWidth="1"/>
-    <col min="6667" max="6667" width="14.625" style="7" customWidth="1"/>
-    <col min="6668" max="6668" width="19.75" style="7" customWidth="1"/>
-    <col min="6669" max="6912" width="9" style="7"/>
-    <col min="6913" max="6913" width="11.5" style="7" customWidth="1"/>
-    <col min="6914" max="6914" width="21.375" style="7" customWidth="1"/>
-    <col min="6915" max="6915" width="18.625" style="7" customWidth="1"/>
-    <col min="6916" max="6916" width="23.125" style="7" customWidth="1"/>
-    <col min="6917" max="6917" width="20.875" style="7" customWidth="1"/>
-    <col min="6918" max="6918" width="21.125" style="7" customWidth="1"/>
-    <col min="6919" max="6919" width="13" style="7" customWidth="1"/>
-    <col min="6920" max="6921" width="19.75" style="7" customWidth="1"/>
-    <col min="6922" max="6922" width="24.75" style="7" customWidth="1"/>
-    <col min="6923" max="6923" width="14.625" style="7" customWidth="1"/>
-    <col min="6924" max="6924" width="19.75" style="7" customWidth="1"/>
-    <col min="6925" max="7168" width="9" style="7"/>
-    <col min="7169" max="7169" width="11.5" style="7" customWidth="1"/>
-    <col min="7170" max="7170" width="21.375" style="7" customWidth="1"/>
-    <col min="7171" max="7171" width="18.625" style="7" customWidth="1"/>
-    <col min="7172" max="7172" width="23.125" style="7" customWidth="1"/>
-    <col min="7173" max="7173" width="20.875" style="7" customWidth="1"/>
-    <col min="7174" max="7174" width="21.125" style="7" customWidth="1"/>
-    <col min="7175" max="7175" width="13" style="7" customWidth="1"/>
-    <col min="7176" max="7177" width="19.75" style="7" customWidth="1"/>
-    <col min="7178" max="7178" width="24.75" style="7" customWidth="1"/>
-    <col min="7179" max="7179" width="14.625" style="7" customWidth="1"/>
-    <col min="7180" max="7180" width="19.75" style="7" customWidth="1"/>
-    <col min="7181" max="7424" width="9" style="7"/>
-    <col min="7425" max="7425" width="11.5" style="7" customWidth="1"/>
-    <col min="7426" max="7426" width="21.375" style="7" customWidth="1"/>
-    <col min="7427" max="7427" width="18.625" style="7" customWidth="1"/>
-    <col min="7428" max="7428" width="23.125" style="7" customWidth="1"/>
-    <col min="7429" max="7429" width="20.875" style="7" customWidth="1"/>
-    <col min="7430" max="7430" width="21.125" style="7" customWidth="1"/>
-    <col min="7431" max="7431" width="13" style="7" customWidth="1"/>
-    <col min="7432" max="7433" width="19.75" style="7" customWidth="1"/>
-    <col min="7434" max="7434" width="24.75" style="7" customWidth="1"/>
-    <col min="7435" max="7435" width="14.625" style="7" customWidth="1"/>
-    <col min="7436" max="7436" width="19.75" style="7" customWidth="1"/>
-    <col min="7437" max="7680" width="9" style="7"/>
-    <col min="7681" max="7681" width="11.5" style="7" customWidth="1"/>
-    <col min="7682" max="7682" width="21.375" style="7" customWidth="1"/>
-    <col min="7683" max="7683" width="18.625" style="7" customWidth="1"/>
-    <col min="7684" max="7684" width="23.125" style="7" customWidth="1"/>
-    <col min="7685" max="7685" width="20.875" style="7" customWidth="1"/>
-    <col min="7686" max="7686" width="21.125" style="7" customWidth="1"/>
-    <col min="7687" max="7687" width="13" style="7" customWidth="1"/>
-    <col min="7688" max="7689" width="19.75" style="7" customWidth="1"/>
-    <col min="7690" max="7690" width="24.75" style="7" customWidth="1"/>
-    <col min="7691" max="7691" width="14.625" style="7" customWidth="1"/>
-    <col min="7692" max="7692" width="19.75" style="7" customWidth="1"/>
-    <col min="7693" max="7936" width="9" style="7"/>
-    <col min="7937" max="7937" width="11.5" style="7" customWidth="1"/>
-    <col min="7938" max="7938" width="21.375" style="7" customWidth="1"/>
-    <col min="7939" max="7939" width="18.625" style="7" customWidth="1"/>
-    <col min="7940" max="7940" width="23.125" style="7" customWidth="1"/>
-    <col min="7941" max="7941" width="20.875" style="7" customWidth="1"/>
-    <col min="7942" max="7942" width="21.125" style="7" customWidth="1"/>
-    <col min="7943" max="7943" width="13" style="7" customWidth="1"/>
-    <col min="7944" max="7945" width="19.75" style="7" customWidth="1"/>
-    <col min="7946" max="7946" width="24.75" style="7" customWidth="1"/>
-    <col min="7947" max="7947" width="14.625" style="7" customWidth="1"/>
-    <col min="7948" max="7948" width="19.75" style="7" customWidth="1"/>
-    <col min="7949" max="8192" width="9" style="7"/>
-    <col min="8193" max="8193" width="11.5" style="7" customWidth="1"/>
-    <col min="8194" max="8194" width="21.375" style="7" customWidth="1"/>
-    <col min="8195" max="8195" width="18.625" style="7" customWidth="1"/>
-    <col min="8196" max="8196" width="23.125" style="7" customWidth="1"/>
-    <col min="8197" max="8197" width="20.875" style="7" customWidth="1"/>
-    <col min="8198" max="8198" width="21.125" style="7" customWidth="1"/>
-    <col min="8199" max="8199" width="13" style="7" customWidth="1"/>
-    <col min="8200" max="8201" width="19.75" style="7" customWidth="1"/>
-    <col min="8202" max="8202" width="24.75" style="7" customWidth="1"/>
-    <col min="8203" max="8203" width="14.625" style="7" customWidth="1"/>
-    <col min="8204" max="8204" width="19.75" style="7" customWidth="1"/>
-    <col min="8205" max="8448" width="9" style="7"/>
-    <col min="8449" max="8449" width="11.5" style="7" customWidth="1"/>
-    <col min="8450" max="8450" width="21.375" style="7" customWidth="1"/>
-    <col min="8451" max="8451" width="18.625" style="7" customWidth="1"/>
-    <col min="8452" max="8452" width="23.125" style="7" customWidth="1"/>
-    <col min="8453" max="8453" width="20.875" style="7" customWidth="1"/>
-    <col min="8454" max="8454" width="21.125" style="7" customWidth="1"/>
-    <col min="8455" max="8455" width="13" style="7" customWidth="1"/>
-    <col min="8456" max="8457" width="19.75" style="7" customWidth="1"/>
-    <col min="8458" max="8458" width="24.75" style="7" customWidth="1"/>
-    <col min="8459" max="8459" width="14.625" style="7" customWidth="1"/>
-    <col min="8460" max="8460" width="19.75" style="7" customWidth="1"/>
-    <col min="8461" max="8704" width="9" style="7"/>
-    <col min="8705" max="8705" width="11.5" style="7" customWidth="1"/>
-    <col min="8706" max="8706" width="21.375" style="7" customWidth="1"/>
-    <col min="8707" max="8707" width="18.625" style="7" customWidth="1"/>
-    <col min="8708" max="8708" width="23.125" style="7" customWidth="1"/>
-    <col min="8709" max="8709" width="20.875" style="7" customWidth="1"/>
-    <col min="8710" max="8710" width="21.125" style="7" customWidth="1"/>
-    <col min="8711" max="8711" width="13" style="7" customWidth="1"/>
-    <col min="8712" max="8713" width="19.75" style="7" customWidth="1"/>
-    <col min="8714" max="8714" width="24.75" style="7" customWidth="1"/>
-    <col min="8715" max="8715" width="14.625" style="7" customWidth="1"/>
-    <col min="8716" max="8716" width="19.75" style="7" customWidth="1"/>
-    <col min="8717" max="8960" width="9" style="7"/>
-    <col min="8961" max="8961" width="11.5" style="7" customWidth="1"/>
-    <col min="8962" max="8962" width="21.375" style="7" customWidth="1"/>
-    <col min="8963" max="8963" width="18.625" style="7" customWidth="1"/>
-    <col min="8964" max="8964" width="23.125" style="7" customWidth="1"/>
-    <col min="8965" max="8965" width="20.875" style="7" customWidth="1"/>
-    <col min="8966" max="8966" width="21.125" style="7" customWidth="1"/>
-    <col min="8967" max="8967" width="13" style="7" customWidth="1"/>
-    <col min="8968" max="8969" width="19.75" style="7" customWidth="1"/>
-    <col min="8970" max="8970" width="24.75" style="7" customWidth="1"/>
-    <col min="8971" max="8971" width="14.625" style="7" customWidth="1"/>
-    <col min="8972" max="8972" width="19.75" style="7" customWidth="1"/>
-    <col min="8973" max="9216" width="9" style="7"/>
-    <col min="9217" max="9217" width="11.5" style="7" customWidth="1"/>
-    <col min="9218" max="9218" width="21.375" style="7" customWidth="1"/>
-    <col min="9219" max="9219" width="18.625" style="7" customWidth="1"/>
-    <col min="9220" max="9220" width="23.125" style="7" customWidth="1"/>
-    <col min="9221" max="9221" width="20.875" style="7" customWidth="1"/>
-    <col min="9222" max="9222" width="21.125" style="7" customWidth="1"/>
-    <col min="9223" max="9223" width="13" style="7" customWidth="1"/>
-    <col min="9224" max="9225" width="19.75" style="7" customWidth="1"/>
-    <col min="9226" max="9226" width="24.75" style="7" customWidth="1"/>
-    <col min="9227" max="9227" width="14.625" style="7" customWidth="1"/>
-    <col min="9228" max="9228" width="19.75" style="7" customWidth="1"/>
-    <col min="9229" max="9472" width="9" style="7"/>
-    <col min="9473" max="9473" width="11.5" style="7" customWidth="1"/>
-    <col min="9474" max="9474" width="21.375" style="7" customWidth="1"/>
-    <col min="9475" max="9475" width="18.625" style="7" customWidth="1"/>
-    <col min="9476" max="9476" width="23.125" style="7" customWidth="1"/>
-    <col min="9477" max="9477" width="20.875" style="7" customWidth="1"/>
-    <col min="9478" max="9478" width="21.125" style="7" customWidth="1"/>
-    <col min="9479" max="9479" width="13" style="7" customWidth="1"/>
-    <col min="9480" max="9481" width="19.75" style="7" customWidth="1"/>
-    <col min="9482" max="9482" width="24.75" style="7" customWidth="1"/>
-    <col min="9483" max="9483" width="14.625" style="7" customWidth="1"/>
-    <col min="9484" max="9484" width="19.75" style="7" customWidth="1"/>
-    <col min="9485" max="9728" width="9" style="7"/>
-    <col min="9729" max="9729" width="11.5" style="7" customWidth="1"/>
-    <col min="9730" max="9730" width="21.375" style="7" customWidth="1"/>
-    <col min="9731" max="9731" width="18.625" style="7" customWidth="1"/>
-    <col min="9732" max="9732" width="23.125" style="7" customWidth="1"/>
-    <col min="9733" max="9733" width="20.875" style="7" customWidth="1"/>
-    <col min="9734" max="9734" width="21.125" style="7" customWidth="1"/>
-    <col min="9735" max="9735" width="13" style="7" customWidth="1"/>
-    <col min="9736" max="9737" width="19.75" style="7" customWidth="1"/>
-    <col min="9738" max="9738" width="24.75" style="7" customWidth="1"/>
-    <col min="9739" max="9739" width="14.625" style="7" customWidth="1"/>
-    <col min="9740" max="9740" width="19.75" style="7" customWidth="1"/>
-    <col min="9741" max="9984" width="9" style="7"/>
-    <col min="9985" max="9985" width="11.5" style="7" customWidth="1"/>
-    <col min="9986" max="9986" width="21.375" style="7" customWidth="1"/>
-    <col min="9987" max="9987" width="18.625" style="7" customWidth="1"/>
-    <col min="9988" max="9988" width="23.125" style="7" customWidth="1"/>
-    <col min="9989" max="9989" width="20.875" style="7" customWidth="1"/>
-    <col min="9990" max="9990" width="21.125" style="7" customWidth="1"/>
-    <col min="9991" max="9991" width="13" style="7" customWidth="1"/>
-    <col min="9992" max="9993" width="19.75" style="7" customWidth="1"/>
-    <col min="9994" max="9994" width="24.75" style="7" customWidth="1"/>
-    <col min="9995" max="9995" width="14.625" style="7" customWidth="1"/>
-    <col min="9996" max="9996" width="19.75" style="7" customWidth="1"/>
-    <col min="9997" max="10240" width="9" style="7"/>
-    <col min="10241" max="10241" width="11.5" style="7" customWidth="1"/>
-    <col min="10242" max="10242" width="21.375" style="7" customWidth="1"/>
-    <col min="10243" max="10243" width="18.625" style="7" customWidth="1"/>
-    <col min="10244" max="10244" width="23.125" style="7" customWidth="1"/>
-    <col min="10245" max="10245" width="20.875" style="7" customWidth="1"/>
-    <col min="10246" max="10246" width="21.125" style="7" customWidth="1"/>
-    <col min="10247" max="10247" width="13" style="7" customWidth="1"/>
-    <col min="10248" max="10249" width="19.75" style="7" customWidth="1"/>
-    <col min="10250" max="10250" width="24.75" style="7" customWidth="1"/>
-    <col min="10251" max="10251" width="14.625" style="7" customWidth="1"/>
-    <col min="10252" max="10252" width="19.75" style="7" customWidth="1"/>
-    <col min="10253" max="10496" width="9" style="7"/>
-    <col min="10497" max="10497" width="11.5" style="7" customWidth="1"/>
-    <col min="10498" max="10498" width="21.375" style="7" customWidth="1"/>
-    <col min="10499" max="10499" width="18.625" style="7" customWidth="1"/>
-    <col min="10500" max="10500" width="23.125" style="7" customWidth="1"/>
-    <col min="10501" max="10501" width="20.875" style="7" customWidth="1"/>
-    <col min="10502" max="10502" width="21.125" style="7" customWidth="1"/>
-    <col min="10503" max="10503" width="13" style="7" customWidth="1"/>
-    <col min="10504" max="10505" width="19.75" style="7" customWidth="1"/>
-    <col min="10506" max="10506" width="24.75" style="7" customWidth="1"/>
-    <col min="10507" max="10507" width="14.625" style="7" customWidth="1"/>
-    <col min="10508" max="10508" width="19.75" style="7" customWidth="1"/>
-    <col min="10509" max="10752" width="9" style="7"/>
-    <col min="10753" max="10753" width="11.5" style="7" customWidth="1"/>
-    <col min="10754" max="10754" width="21.375" style="7" customWidth="1"/>
-    <col min="10755" max="10755" width="18.625" style="7" customWidth="1"/>
-    <col min="10756" max="10756" width="23.125" style="7" customWidth="1"/>
-    <col min="10757" max="10757" width="20.875" style="7" customWidth="1"/>
-    <col min="10758" max="10758" width="21.125" style="7" customWidth="1"/>
-    <col min="10759" max="10759" width="13" style="7" customWidth="1"/>
-    <col min="10760" max="10761" width="19.75" style="7" customWidth="1"/>
-    <col min="10762" max="10762" width="24.75" style="7" customWidth="1"/>
-    <col min="10763" max="10763" width="14.625" style="7" customWidth="1"/>
-    <col min="10764" max="10764" width="19.75" style="7" customWidth="1"/>
-    <col min="10765" max="11008" width="9" style="7"/>
-    <col min="11009" max="11009" width="11.5" style="7" customWidth="1"/>
-    <col min="11010" max="11010" width="21.375" style="7" customWidth="1"/>
-    <col min="11011" max="11011" width="18.625" style="7" customWidth="1"/>
-    <col min="11012" max="11012" width="23.125" style="7" customWidth="1"/>
-    <col min="11013" max="11013" width="20.875" style="7" customWidth="1"/>
-    <col min="11014" max="11014" width="21.125" style="7" customWidth="1"/>
-    <col min="11015" max="11015" width="13" style="7" customWidth="1"/>
-    <col min="11016" max="11017" width="19.75" style="7" customWidth="1"/>
-    <col min="11018" max="11018" width="24.75" style="7" customWidth="1"/>
-    <col min="11019" max="11019" width="14.625" style="7" customWidth="1"/>
-    <col min="11020" max="11020" width="19.75" style="7" customWidth="1"/>
-    <col min="11021" max="11264" width="9" style="7"/>
-    <col min="11265" max="11265" width="11.5" style="7" customWidth="1"/>
-    <col min="11266" max="11266" width="21.375" style="7" customWidth="1"/>
-    <col min="11267" max="11267" width="18.625" style="7" customWidth="1"/>
-    <col min="11268" max="11268" width="23.125" style="7" customWidth="1"/>
-    <col min="11269" max="11269" width="20.875" style="7" customWidth="1"/>
-    <col min="11270" max="11270" width="21.125" style="7" customWidth="1"/>
-    <col min="11271" max="11271" width="13" style="7" customWidth="1"/>
-    <col min="11272" max="11273" width="19.75" style="7" customWidth="1"/>
-    <col min="11274" max="11274" width="24.75" style="7" customWidth="1"/>
-    <col min="11275" max="11275" width="14.625" style="7" customWidth="1"/>
-    <col min="11276" max="11276" width="19.75" style="7" customWidth="1"/>
-    <col min="11277" max="11520" width="9" style="7"/>
-    <col min="11521" max="11521" width="11.5" style="7" customWidth="1"/>
-    <col min="11522" max="11522" width="21.375" style="7" customWidth="1"/>
-    <col min="11523" max="11523" width="18.625" style="7" customWidth="1"/>
-    <col min="11524" max="11524" width="23.125" style="7" customWidth="1"/>
-    <col min="11525" max="11525" width="20.875" style="7" customWidth="1"/>
-    <col min="11526" max="11526" width="21.125" style="7" customWidth="1"/>
-    <col min="11527" max="11527" width="13" style="7" customWidth="1"/>
-    <col min="11528" max="11529" width="19.75" style="7" customWidth="1"/>
-    <col min="11530" max="11530" width="24.75" style="7" customWidth="1"/>
-    <col min="11531" max="11531" width="14.625" style="7" customWidth="1"/>
-    <col min="11532" max="11532" width="19.75" style="7" customWidth="1"/>
-    <col min="11533" max="11776" width="9" style="7"/>
-    <col min="11777" max="11777" width="11.5" style="7" customWidth="1"/>
-    <col min="11778" max="11778" width="21.375" style="7" customWidth="1"/>
-    <col min="11779" max="11779" width="18.625" style="7" customWidth="1"/>
-    <col min="11780" max="11780" width="23.125" style="7" customWidth="1"/>
-    <col min="11781" max="11781" width="20.875" style="7" customWidth="1"/>
-    <col min="11782" max="11782" width="21.125" style="7" customWidth="1"/>
-    <col min="11783" max="11783" width="13" style="7" customWidth="1"/>
-    <col min="11784" max="11785" width="19.75" style="7" customWidth="1"/>
-    <col min="11786" max="11786" width="24.75" style="7" customWidth="1"/>
-    <col min="11787" max="11787" width="14.625" style="7" customWidth="1"/>
-    <col min="11788" max="11788" width="19.75" style="7" customWidth="1"/>
-    <col min="11789" max="12032" width="9" style="7"/>
-    <col min="12033" max="12033" width="11.5" style="7" customWidth="1"/>
-    <col min="12034" max="12034" width="21.375" style="7" customWidth="1"/>
-    <col min="12035" max="12035" width="18.625" style="7" customWidth="1"/>
-    <col min="12036" max="12036" width="23.125" style="7" customWidth="1"/>
-    <col min="12037" max="12037" width="20.875" style="7" customWidth="1"/>
-    <col min="12038" max="12038" width="21.125" style="7" customWidth="1"/>
-    <col min="12039" max="12039" width="13" style="7" customWidth="1"/>
-    <col min="12040" max="12041" width="19.75" style="7" customWidth="1"/>
-    <col min="12042" max="12042" width="24.75" style="7" customWidth="1"/>
-    <col min="12043" max="12043" width="14.625" style="7" customWidth="1"/>
-    <col min="12044" max="12044" width="19.75" style="7" customWidth="1"/>
-    <col min="12045" max="12288" width="9" style="7"/>
-    <col min="12289" max="12289" width="11.5" style="7" customWidth="1"/>
-    <col min="12290" max="12290" width="21.375" style="7" customWidth="1"/>
-    <col min="12291" max="12291" width="18.625" style="7" customWidth="1"/>
-    <col min="12292" max="12292" width="23.125" style="7" customWidth="1"/>
-    <col min="12293" max="12293" width="20.875" style="7" customWidth="1"/>
-    <col min="12294" max="12294" width="21.125" style="7" customWidth="1"/>
-    <col min="12295" max="12295" width="13" style="7" customWidth="1"/>
-    <col min="12296" max="12297" width="19.75" style="7" customWidth="1"/>
-    <col min="12298" max="12298" width="24.75" style="7" customWidth="1"/>
-    <col min="12299" max="12299" width="14.625" style="7" customWidth="1"/>
-    <col min="12300" max="12300" width="19.75" style="7" customWidth="1"/>
-    <col min="12301" max="12544" width="9" style="7"/>
-    <col min="12545" max="12545" width="11.5" style="7" customWidth="1"/>
-    <col min="12546" max="12546" width="21.375" style="7" customWidth="1"/>
-    <col min="12547" max="12547" width="18.625" style="7" customWidth="1"/>
-    <col min="12548" max="12548" width="23.125" style="7" customWidth="1"/>
-    <col min="12549" max="12549" width="20.875" style="7" customWidth="1"/>
-    <col min="12550" max="12550" width="21.125" style="7" customWidth="1"/>
-    <col min="12551" max="12551" width="13" style="7" customWidth="1"/>
-    <col min="12552" max="12553" width="19.75" style="7" customWidth="1"/>
-    <col min="12554" max="12554" width="24.75" style="7" customWidth="1"/>
-    <col min="12555" max="12555" width="14.625" style="7" customWidth="1"/>
-    <col min="12556" max="12556" width="19.75" style="7" customWidth="1"/>
-    <col min="12557" max="12800" width="9" style="7"/>
-    <col min="12801" max="12801" width="11.5" style="7" customWidth="1"/>
-    <col min="12802" max="12802" width="21.375" style="7" customWidth="1"/>
-    <col min="12803" max="12803" width="18.625" style="7" customWidth="1"/>
-    <col min="12804" max="12804" width="23.125" style="7" customWidth="1"/>
-    <col min="12805" max="12805" width="20.875" style="7" customWidth="1"/>
-    <col min="12806" max="12806" width="21.125" style="7" customWidth="1"/>
-    <col min="12807" max="12807" width="13" style="7" customWidth="1"/>
-    <col min="12808" max="12809" width="19.75" style="7" customWidth="1"/>
-    <col min="12810" max="12810" width="24.75" style="7" customWidth="1"/>
-    <col min="12811" max="12811" width="14.625" style="7" customWidth="1"/>
-    <col min="12812" max="12812" width="19.75" style="7" customWidth="1"/>
-    <col min="12813" max="13056" width="9" style="7"/>
-    <col min="13057" max="13057" width="11.5" style="7" customWidth="1"/>
-    <col min="13058" max="13058" width="21.375" style="7" customWidth="1"/>
-    <col min="13059" max="13059" width="18.625" style="7" customWidth="1"/>
-    <col min="13060" max="13060" width="23.125" style="7" customWidth="1"/>
-    <col min="13061" max="13061" width="20.875" style="7" customWidth="1"/>
-    <col min="13062" max="13062" width="21.125" style="7" customWidth="1"/>
-    <col min="13063" max="13063" width="13" style="7" customWidth="1"/>
-    <col min="13064" max="13065" width="19.75" style="7" customWidth="1"/>
-    <col min="13066" max="13066" width="24.75" style="7" customWidth="1"/>
-    <col min="13067" max="13067" width="14.625" style="7" customWidth="1"/>
-    <col min="13068" max="13068" width="19.75" style="7" customWidth="1"/>
-    <col min="13069" max="13312" width="9" style="7"/>
-    <col min="13313" max="13313" width="11.5" style="7" customWidth="1"/>
-    <col min="13314" max="13314" width="21.375" style="7" customWidth="1"/>
-    <col min="13315" max="13315" width="18.625" style="7" customWidth="1"/>
-    <col min="13316" max="13316" width="23.125" style="7" customWidth="1"/>
-    <col min="13317" max="13317" width="20.875" style="7" customWidth="1"/>
-    <col min="13318" max="13318" width="21.125" style="7" customWidth="1"/>
-    <col min="13319" max="13319" width="13" style="7" customWidth="1"/>
-    <col min="13320" max="13321" width="19.75" style="7" customWidth="1"/>
-    <col min="13322" max="13322" width="24.75" style="7" customWidth="1"/>
-    <col min="13323" max="13323" width="14.625" style="7" customWidth="1"/>
-    <col min="13324" max="13324" width="19.75" style="7" customWidth="1"/>
-    <col min="13325" max="13568" width="9" style="7"/>
-    <col min="13569" max="13569" width="11.5" style="7" customWidth="1"/>
-    <col min="13570" max="13570" width="21.375" style="7" customWidth="1"/>
-    <col min="13571" max="13571" width="18.625" style="7" customWidth="1"/>
-    <col min="13572" max="13572" width="23.125" style="7" customWidth="1"/>
-    <col min="13573" max="13573" width="20.875" style="7" customWidth="1"/>
-    <col min="13574" max="13574" width="21.125" style="7" customWidth="1"/>
-    <col min="13575" max="13575" width="13" style="7" customWidth="1"/>
-    <col min="13576" max="13577" width="19.75" style="7" customWidth="1"/>
-    <col min="13578" max="13578" width="24.75" style="7" customWidth="1"/>
-    <col min="13579" max="13579" width="14.625" style="7" customWidth="1"/>
-    <col min="13580" max="13580" width="19.75" style="7" customWidth="1"/>
-    <col min="13581" max="13824" width="9" style="7"/>
-    <col min="13825" max="13825" width="11.5" style="7" customWidth="1"/>
-    <col min="13826" max="13826" width="21.375" style="7" customWidth="1"/>
-    <col min="13827" max="13827" width="18.625" style="7" customWidth="1"/>
-    <col min="13828" max="13828" width="23.125" style="7" customWidth="1"/>
-    <col min="13829" max="13829" width="20.875" style="7" customWidth="1"/>
-    <col min="13830" max="13830" width="21.125" style="7" customWidth="1"/>
-    <col min="13831" max="13831" width="13" style="7" customWidth="1"/>
-    <col min="13832" max="13833" width="19.75" style="7" customWidth="1"/>
-    <col min="13834" max="13834" width="24.75" style="7" customWidth="1"/>
-    <col min="13835" max="13835" width="14.625" style="7" customWidth="1"/>
-    <col min="13836" max="13836" width="19.75" style="7" customWidth="1"/>
-    <col min="13837" max="14080" width="9" style="7"/>
-    <col min="14081" max="14081" width="11.5" style="7" customWidth="1"/>
-    <col min="14082" max="14082" width="21.375" style="7" customWidth="1"/>
-    <col min="14083" max="14083" width="18.625" style="7" customWidth="1"/>
-    <col min="14084" max="14084" width="23.125" style="7" customWidth="1"/>
-    <col min="14085" max="14085" width="20.875" style="7" customWidth="1"/>
-    <col min="14086" max="14086" width="21.125" style="7" customWidth="1"/>
-    <col min="14087" max="14087" width="13" style="7" customWidth="1"/>
-    <col min="14088" max="14089" width="19.75" style="7" customWidth="1"/>
-    <col min="14090" max="14090" width="24.75" style="7" customWidth="1"/>
-    <col min="14091" max="14091" width="14.625" style="7" customWidth="1"/>
-    <col min="14092" max="14092" width="19.75" style="7" customWidth="1"/>
-    <col min="14093" max="14336" width="9" style="7"/>
-    <col min="14337" max="14337" width="11.5" style="7" customWidth="1"/>
-    <col min="14338" max="14338" width="21.375" style="7" customWidth="1"/>
-    <col min="14339" max="14339" width="18.625" style="7" customWidth="1"/>
-    <col min="14340" max="14340" width="23.125" style="7" customWidth="1"/>
-    <col min="14341" max="14341" width="20.875" style="7" customWidth="1"/>
-    <col min="14342" max="14342" width="21.125" style="7" customWidth="1"/>
-    <col min="14343" max="14343" width="13" style="7" customWidth="1"/>
-    <col min="14344" max="14345" width="19.75" style="7" customWidth="1"/>
-    <col min="14346" max="14346" width="24.75" style="7" customWidth="1"/>
-    <col min="14347" max="14347" width="14.625" style="7" customWidth="1"/>
-    <col min="14348" max="14348" width="19.75" style="7" customWidth="1"/>
-    <col min="14349" max="14592" width="9" style="7"/>
-    <col min="14593" max="14593" width="11.5" style="7" customWidth="1"/>
-    <col min="14594" max="14594" width="21.375" style="7" customWidth="1"/>
-    <col min="14595" max="14595" width="18.625" style="7" customWidth="1"/>
-    <col min="14596" max="14596" width="23.125" style="7" customWidth="1"/>
-    <col min="14597" max="14597" width="20.875" style="7" customWidth="1"/>
-    <col min="14598" max="14598" width="21.125" style="7" customWidth="1"/>
-    <col min="14599" max="14599" width="13" style="7" customWidth="1"/>
-    <col min="14600" max="14601" width="19.75" style="7" customWidth="1"/>
-    <col min="14602" max="14602" width="24.75" style="7" customWidth="1"/>
-    <col min="14603" max="14603" width="14.625" style="7" customWidth="1"/>
-    <col min="14604" max="14604" width="19.75" style="7" customWidth="1"/>
-    <col min="14605" max="14848" width="9" style="7"/>
-    <col min="14849" max="14849" width="11.5" style="7" customWidth="1"/>
-    <col min="14850" max="14850" width="21.375" style="7" customWidth="1"/>
-    <col min="14851" max="14851" width="18.625" style="7" customWidth="1"/>
-    <col min="14852" max="14852" width="23.125" style="7" customWidth="1"/>
-    <col min="14853" max="14853" width="20.875" style="7" customWidth="1"/>
-    <col min="14854" max="14854" width="21.125" style="7" customWidth="1"/>
-    <col min="14855" max="14855" width="13" style="7" customWidth="1"/>
-    <col min="14856" max="14857" width="19.75" style="7" customWidth="1"/>
-    <col min="14858" max="14858" width="24.75" style="7" customWidth="1"/>
-    <col min="14859" max="14859" width="14.625" style="7" customWidth="1"/>
-    <col min="14860" max="14860" width="19.75" style="7" customWidth="1"/>
-    <col min="14861" max="15104" width="9" style="7"/>
-    <col min="15105" max="15105" width="11.5" style="7" customWidth="1"/>
-    <col min="15106" max="15106" width="21.375" style="7" customWidth="1"/>
-    <col min="15107" max="15107" width="18.625" style="7" customWidth="1"/>
-    <col min="15108" max="15108" width="23.125" style="7" customWidth="1"/>
-    <col min="15109" max="15109" width="20.875" style="7" customWidth="1"/>
-    <col min="15110" max="15110" width="21.125" style="7" customWidth="1"/>
-    <col min="15111" max="15111" width="13" style="7" customWidth="1"/>
-    <col min="15112" max="15113" width="19.75" style="7" customWidth="1"/>
-    <col min="15114" max="15114" width="24.75" style="7" customWidth="1"/>
-    <col min="15115" max="15115" width="14.625" style="7" customWidth="1"/>
-    <col min="15116" max="15116" width="19.75" style="7" customWidth="1"/>
-    <col min="15117" max="15360" width="9" style="7"/>
-    <col min="15361" max="15361" width="11.5" style="7" customWidth="1"/>
-    <col min="15362" max="15362" width="21.375" style="7" customWidth="1"/>
-    <col min="15363" max="15363" width="18.625" style="7" customWidth="1"/>
-    <col min="15364" max="15364" width="23.125" style="7" customWidth="1"/>
-    <col min="15365" max="15365" width="20.875" style="7" customWidth="1"/>
-    <col min="15366" max="15366" width="21.125" style="7" customWidth="1"/>
-    <col min="15367" max="15367" width="13" style="7" customWidth="1"/>
-    <col min="15368" max="15369" width="19.75" style="7" customWidth="1"/>
-    <col min="15370" max="15370" width="24.75" style="7" customWidth="1"/>
-    <col min="15371" max="15371" width="14.625" style="7" customWidth="1"/>
-    <col min="15372" max="15372" width="19.75" style="7" customWidth="1"/>
-    <col min="15373" max="15616" width="9" style="7"/>
-    <col min="15617" max="15617" width="11.5" style="7" customWidth="1"/>
-    <col min="15618" max="15618" width="21.375" style="7" customWidth="1"/>
-    <col min="15619" max="15619" width="18.625" style="7" customWidth="1"/>
-    <col min="15620" max="15620" width="23.125" style="7" customWidth="1"/>
-    <col min="15621" max="15621" width="20.875" style="7" customWidth="1"/>
-    <col min="15622" max="15622" width="21.125" style="7" customWidth="1"/>
-    <col min="15623" max="15623" width="13" style="7" customWidth="1"/>
-    <col min="15624" max="15625" width="19.75" style="7" customWidth="1"/>
-    <col min="15626" max="15626" width="24.75" style="7" customWidth="1"/>
-    <col min="15627" max="15627" width="14.625" style="7" customWidth="1"/>
-    <col min="15628" max="15628" width="19.75" style="7" customWidth="1"/>
-    <col min="15629" max="15872" width="9" style="7"/>
-    <col min="15873" max="15873" width="11.5" style="7" customWidth="1"/>
-    <col min="15874" max="15874" width="21.375" style="7" customWidth="1"/>
-    <col min="15875" max="15875" width="18.625" style="7" customWidth="1"/>
-    <col min="15876" max="15876" width="23.125" style="7" customWidth="1"/>
-    <col min="15877" max="15877" width="20.875" style="7" customWidth="1"/>
-    <col min="15878" max="15878" width="21.125" style="7" customWidth="1"/>
-    <col min="15879" max="15879" width="13" style="7" customWidth="1"/>
-    <col min="15880" max="15881" width="19.75" style="7" customWidth="1"/>
-    <col min="15882" max="15882" width="24.75" style="7" customWidth="1"/>
-    <col min="15883" max="15883" width="14.625" style="7" customWidth="1"/>
-    <col min="15884" max="15884" width="19.75" style="7" customWidth="1"/>
-    <col min="15885" max="16128" width="9" style="7"/>
-    <col min="16129" max="16129" width="11.5" style="7" customWidth="1"/>
-    <col min="16130" max="16130" width="21.375" style="7" customWidth="1"/>
-    <col min="16131" max="16131" width="18.625" style="7" customWidth="1"/>
-    <col min="16132" max="16132" width="23.125" style="7" customWidth="1"/>
-    <col min="16133" max="16133" width="20.875" style="7" customWidth="1"/>
-    <col min="16134" max="16134" width="21.125" style="7" customWidth="1"/>
-    <col min="16135" max="16135" width="13" style="7" customWidth="1"/>
-    <col min="16136" max="16137" width="19.75" style="7" customWidth="1"/>
-    <col min="16138" max="16138" width="24.75" style="7" customWidth="1"/>
-    <col min="16139" max="16139" width="14.625" style="7" customWidth="1"/>
-    <col min="16140" max="16140" width="19.75" style="7" customWidth="1"/>
-    <col min="16141" max="16384" width="9" style="7"/>
+    <col min="1" max="1" width="11.5" style="4" customWidth="1"/>
+    <col min="2" max="2" width="21.375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="18.625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="23.125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="20.875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="21.125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="13" style="4" customWidth="1"/>
+    <col min="8" max="9" width="19.75" style="4" customWidth="1"/>
+    <col min="10" max="10" width="24.75" style="4" customWidth="1"/>
+    <col min="11" max="11" width="14.625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="19.75" style="4" customWidth="1"/>
+    <col min="13" max="256" width="9" style="4"/>
+    <col min="257" max="257" width="11.5" style="4" customWidth="1"/>
+    <col min="258" max="258" width="21.375" style="4" customWidth="1"/>
+    <col min="259" max="259" width="18.625" style="4" customWidth="1"/>
+    <col min="260" max="260" width="23.125" style="4" customWidth="1"/>
+    <col min="261" max="261" width="20.875" style="4" customWidth="1"/>
+    <col min="262" max="262" width="21.125" style="4" customWidth="1"/>
+    <col min="263" max="263" width="13" style="4" customWidth="1"/>
+    <col min="264" max="265" width="19.75" style="4" customWidth="1"/>
+    <col min="266" max="266" width="24.75" style="4" customWidth="1"/>
+    <col min="267" max="267" width="14.625" style="4" customWidth="1"/>
+    <col min="268" max="268" width="19.75" style="4" customWidth="1"/>
+    <col min="269" max="512" width="9" style="4"/>
+    <col min="513" max="513" width="11.5" style="4" customWidth="1"/>
+    <col min="514" max="514" width="21.375" style="4" customWidth="1"/>
+    <col min="515" max="515" width="18.625" style="4" customWidth="1"/>
+    <col min="516" max="516" width="23.125" style="4" customWidth="1"/>
+    <col min="517" max="517" width="20.875" style="4" customWidth="1"/>
+    <col min="518" max="518" width="21.125" style="4" customWidth="1"/>
+    <col min="519" max="519" width="13" style="4" customWidth="1"/>
+    <col min="520" max="521" width="19.75" style="4" customWidth="1"/>
+    <col min="522" max="522" width="24.75" style="4" customWidth="1"/>
+    <col min="523" max="523" width="14.625" style="4" customWidth="1"/>
+    <col min="524" max="524" width="19.75" style="4" customWidth="1"/>
+    <col min="525" max="768" width="9" style="4"/>
+    <col min="769" max="769" width="11.5" style="4" customWidth="1"/>
+    <col min="770" max="770" width="21.375" style="4" customWidth="1"/>
+    <col min="771" max="771" width="18.625" style="4" customWidth="1"/>
+    <col min="772" max="772" width="23.125" style="4" customWidth="1"/>
+    <col min="773" max="773" width="20.875" style="4" customWidth="1"/>
+    <col min="774" max="774" width="21.125" style="4" customWidth="1"/>
+    <col min="775" max="775" width="13" style="4" customWidth="1"/>
+    <col min="776" max="777" width="19.75" style="4" customWidth="1"/>
+    <col min="778" max="778" width="24.75" style="4" customWidth="1"/>
+    <col min="779" max="779" width="14.625" style="4" customWidth="1"/>
+    <col min="780" max="780" width="19.75" style="4" customWidth="1"/>
+    <col min="781" max="1024" width="9" style="4"/>
+    <col min="1025" max="1025" width="11.5" style="4" customWidth="1"/>
+    <col min="1026" max="1026" width="21.375" style="4" customWidth="1"/>
+    <col min="1027" max="1027" width="18.625" style="4" customWidth="1"/>
+    <col min="1028" max="1028" width="23.125" style="4" customWidth="1"/>
+    <col min="1029" max="1029" width="20.875" style="4" customWidth="1"/>
+    <col min="1030" max="1030" width="21.125" style="4" customWidth="1"/>
+    <col min="1031" max="1031" width="13" style="4" customWidth="1"/>
+    <col min="1032" max="1033" width="19.75" style="4" customWidth="1"/>
+    <col min="1034" max="1034" width="24.75" style="4" customWidth="1"/>
+    <col min="1035" max="1035" width="14.625" style="4" customWidth="1"/>
+    <col min="1036" max="1036" width="19.75" style="4" customWidth="1"/>
+    <col min="1037" max="1280" width="9" style="4"/>
+    <col min="1281" max="1281" width="11.5" style="4" customWidth="1"/>
+    <col min="1282" max="1282" width="21.375" style="4" customWidth="1"/>
+    <col min="1283" max="1283" width="18.625" style="4" customWidth="1"/>
+    <col min="1284" max="1284" width="23.125" style="4" customWidth="1"/>
+    <col min="1285" max="1285" width="20.875" style="4" customWidth="1"/>
+    <col min="1286" max="1286" width="21.125" style="4" customWidth="1"/>
+    <col min="1287" max="1287" width="13" style="4" customWidth="1"/>
+    <col min="1288" max="1289" width="19.75" style="4" customWidth="1"/>
+    <col min="1290" max="1290" width="24.75" style="4" customWidth="1"/>
+    <col min="1291" max="1291" width="14.625" style="4" customWidth="1"/>
+    <col min="1292" max="1292" width="19.75" style="4" customWidth="1"/>
+    <col min="1293" max="1536" width="9" style="4"/>
+    <col min="1537" max="1537" width="11.5" style="4" customWidth="1"/>
+    <col min="1538" max="1538" width="21.375" style="4" customWidth="1"/>
+    <col min="1539" max="1539" width="18.625" style="4" customWidth="1"/>
+    <col min="1540" max="1540" width="23.125" style="4" customWidth="1"/>
+    <col min="1541" max="1541" width="20.875" style="4" customWidth="1"/>
+    <col min="1542" max="1542" width="21.125" style="4" customWidth="1"/>
+    <col min="1543" max="1543" width="13" style="4" customWidth="1"/>
+    <col min="1544" max="1545" width="19.75" style="4" customWidth="1"/>
+    <col min="1546" max="1546" width="24.75" style="4" customWidth="1"/>
+    <col min="1547" max="1547" width="14.625" style="4" customWidth="1"/>
+    <col min="1548" max="1548" width="19.75" style="4" customWidth="1"/>
+    <col min="1549" max="1792" width="9" style="4"/>
+    <col min="1793" max="1793" width="11.5" style="4" customWidth="1"/>
+    <col min="1794" max="1794" width="21.375" style="4" customWidth="1"/>
+    <col min="1795" max="1795" width="18.625" style="4" customWidth="1"/>
+    <col min="1796" max="1796" width="23.125" style="4" customWidth="1"/>
+    <col min="1797" max="1797" width="20.875" style="4" customWidth="1"/>
+    <col min="1798" max="1798" width="21.125" style="4" customWidth="1"/>
+    <col min="1799" max="1799" width="13" style="4" customWidth="1"/>
+    <col min="1800" max="1801" width="19.75" style="4" customWidth="1"/>
+    <col min="1802" max="1802" width="24.75" style="4" customWidth="1"/>
+    <col min="1803" max="1803" width="14.625" style="4" customWidth="1"/>
+    <col min="1804" max="1804" width="19.75" style="4" customWidth="1"/>
+    <col min="1805" max="2048" width="9" style="4"/>
+    <col min="2049" max="2049" width="11.5" style="4" customWidth="1"/>
+    <col min="2050" max="2050" width="21.375" style="4" customWidth="1"/>
+    <col min="2051" max="2051" width="18.625" style="4" customWidth="1"/>
+    <col min="2052" max="2052" width="23.125" style="4" customWidth="1"/>
+    <col min="2053" max="2053" width="20.875" style="4" customWidth="1"/>
+    <col min="2054" max="2054" width="21.125" style="4" customWidth="1"/>
+    <col min="2055" max="2055" width="13" style="4" customWidth="1"/>
+    <col min="2056" max="2057" width="19.75" style="4" customWidth="1"/>
+    <col min="2058" max="2058" width="24.75" style="4" customWidth="1"/>
+    <col min="2059" max="2059" width="14.625" style="4" customWidth="1"/>
+    <col min="2060" max="2060" width="19.75" style="4" customWidth="1"/>
+    <col min="2061" max="2304" width="9" style="4"/>
+    <col min="2305" max="2305" width="11.5" style="4" customWidth="1"/>
+    <col min="2306" max="2306" width="21.375" style="4" customWidth="1"/>
+    <col min="2307" max="2307" width="18.625" style="4" customWidth="1"/>
+    <col min="2308" max="2308" width="23.125" style="4" customWidth="1"/>
+    <col min="2309" max="2309" width="20.875" style="4" customWidth="1"/>
+    <col min="2310" max="2310" width="21.125" style="4" customWidth="1"/>
+    <col min="2311" max="2311" width="13" style="4" customWidth="1"/>
+    <col min="2312" max="2313" width="19.75" style="4" customWidth="1"/>
+    <col min="2314" max="2314" width="24.75" style="4" customWidth="1"/>
+    <col min="2315" max="2315" width="14.625" style="4" customWidth="1"/>
+    <col min="2316" max="2316" width="19.75" style="4" customWidth="1"/>
+    <col min="2317" max="2560" width="9" style="4"/>
+    <col min="2561" max="2561" width="11.5" style="4" customWidth="1"/>
+    <col min="2562" max="2562" width="21.375" style="4" customWidth="1"/>
+    <col min="2563" max="2563" width="18.625" style="4" customWidth="1"/>
+    <col min="2564" max="2564" width="23.125" style="4" customWidth="1"/>
+    <col min="2565" max="2565" width="20.875" style="4" customWidth="1"/>
+    <col min="2566" max="2566" width="21.125" style="4" customWidth="1"/>
+    <col min="2567" max="2567" width="13" style="4" customWidth="1"/>
+    <col min="2568" max="2569" width="19.75" style="4" customWidth="1"/>
+    <col min="2570" max="2570" width="24.75" style="4" customWidth="1"/>
+    <col min="2571" max="2571" width="14.625" style="4" customWidth="1"/>
+    <col min="2572" max="2572" width="19.75" style="4" customWidth="1"/>
+    <col min="2573" max="2816" width="9" style="4"/>
+    <col min="2817" max="2817" width="11.5" style="4" customWidth="1"/>
+    <col min="2818" max="2818" width="21.375" style="4" customWidth="1"/>
+    <col min="2819" max="2819" width="18.625" style="4" customWidth="1"/>
+    <col min="2820" max="2820" width="23.125" style="4" customWidth="1"/>
+    <col min="2821" max="2821" width="20.875" style="4" customWidth="1"/>
+    <col min="2822" max="2822" width="21.125" style="4" customWidth="1"/>
+    <col min="2823" max="2823" width="13" style="4" customWidth="1"/>
+    <col min="2824" max="2825" width="19.75" style="4" customWidth="1"/>
+    <col min="2826" max="2826" width="24.75" style="4" customWidth="1"/>
+    <col min="2827" max="2827" width="14.625" style="4" customWidth="1"/>
+    <col min="2828" max="2828" width="19.75" style="4" customWidth="1"/>
+    <col min="2829" max="3072" width="9" style="4"/>
+    <col min="3073" max="3073" width="11.5" style="4" customWidth="1"/>
+    <col min="3074" max="3074" width="21.375" style="4" customWidth="1"/>
+    <col min="3075" max="3075" width="18.625" style="4" customWidth="1"/>
+    <col min="3076" max="3076" width="23.125" style="4" customWidth="1"/>
+    <col min="3077" max="3077" width="20.875" style="4" customWidth="1"/>
+    <col min="3078" max="3078" width="21.125" style="4" customWidth="1"/>
+    <col min="3079" max="3079" width="13" style="4" customWidth="1"/>
+    <col min="3080" max="3081" width="19.75" style="4" customWidth="1"/>
+    <col min="3082" max="3082" width="24.75" style="4" customWidth="1"/>
+    <col min="3083" max="3083" width="14.625" style="4" customWidth="1"/>
+    <col min="3084" max="3084" width="19.75" style="4" customWidth="1"/>
+    <col min="3085" max="3328" width="9" style="4"/>
+    <col min="3329" max="3329" width="11.5" style="4" customWidth="1"/>
+    <col min="3330" max="3330" width="21.375" style="4" customWidth="1"/>
+    <col min="3331" max="3331" width="18.625" style="4" customWidth="1"/>
+    <col min="3332" max="3332" width="23.125" style="4" customWidth="1"/>
+    <col min="3333" max="3333" width="20.875" style="4" customWidth="1"/>
+    <col min="3334" max="3334" width="21.125" style="4" customWidth="1"/>
+    <col min="3335" max="3335" width="13" style="4" customWidth="1"/>
+    <col min="3336" max="3337" width="19.75" style="4" customWidth="1"/>
+    <col min="3338" max="3338" width="24.75" style="4" customWidth="1"/>
+    <col min="3339" max="3339" width="14.625" style="4" customWidth="1"/>
+    <col min="3340" max="3340" width="19.75" style="4" customWidth="1"/>
+    <col min="3341" max="3584" width="9" style="4"/>
+    <col min="3585" max="3585" width="11.5" style="4" customWidth="1"/>
+    <col min="3586" max="3586" width="21.375" style="4" customWidth="1"/>
+    <col min="3587" max="3587" width="18.625" style="4" customWidth="1"/>
+    <col min="3588" max="3588" width="23.125" style="4" customWidth="1"/>
+    <col min="3589" max="3589" width="20.875" style="4" customWidth="1"/>
+    <col min="3590" max="3590" width="21.125" style="4" customWidth="1"/>
+    <col min="3591" max="3591" width="13" style="4" customWidth="1"/>
+    <col min="3592" max="3593" width="19.75" style="4" customWidth="1"/>
+    <col min="3594" max="3594" width="24.75" style="4" customWidth="1"/>
+    <col min="3595" max="3595" width="14.625" style="4" customWidth="1"/>
+    <col min="3596" max="3596" width="19.75" style="4" customWidth="1"/>
+    <col min="3597" max="3840" width="9" style="4"/>
+    <col min="3841" max="3841" width="11.5" style="4" customWidth="1"/>
+    <col min="3842" max="3842" width="21.375" style="4" customWidth="1"/>
+    <col min="3843" max="3843" width="18.625" style="4" customWidth="1"/>
+    <col min="3844" max="3844" width="23.125" style="4" customWidth="1"/>
+    <col min="3845" max="3845" width="20.875" style="4" customWidth="1"/>
+    <col min="3846" max="3846" width="21.125" style="4" customWidth="1"/>
+    <col min="3847" max="3847" width="13" style="4" customWidth="1"/>
+    <col min="3848" max="3849" width="19.75" style="4" customWidth="1"/>
+    <col min="3850" max="3850" width="24.75" style="4" customWidth="1"/>
+    <col min="3851" max="3851" width="14.625" style="4" customWidth="1"/>
+    <col min="3852" max="3852" width="19.75" style="4" customWidth="1"/>
+    <col min="3853" max="4096" width="9" style="4"/>
+    <col min="4097" max="4097" width="11.5" style="4" customWidth="1"/>
+    <col min="4098" max="4098" width="21.375" style="4" customWidth="1"/>
+    <col min="4099" max="4099" width="18.625" style="4" customWidth="1"/>
+    <col min="4100" max="4100" width="23.125" style="4" customWidth="1"/>
+    <col min="4101" max="4101" width="20.875" style="4" customWidth="1"/>
+    <col min="4102" max="4102" width="21.125" style="4" customWidth="1"/>
+    <col min="4103" max="4103" width="13" style="4" customWidth="1"/>
+    <col min="4104" max="4105" width="19.75" style="4" customWidth="1"/>
+    <col min="4106" max="4106" width="24.75" style="4" customWidth="1"/>
+    <col min="4107" max="4107" width="14.625" style="4" customWidth="1"/>
+    <col min="4108" max="4108" width="19.75" style="4" customWidth="1"/>
+    <col min="4109" max="4352" width="9" style="4"/>
+    <col min="4353" max="4353" width="11.5" style="4" customWidth="1"/>
+    <col min="4354" max="4354" width="21.375" style="4" customWidth="1"/>
+    <col min="4355" max="4355" width="18.625" style="4" customWidth="1"/>
+    <col min="4356" max="4356" width="23.125" style="4" customWidth="1"/>
+    <col min="4357" max="4357" width="20.875" style="4" customWidth="1"/>
+    <col min="4358" max="4358" width="21.125" style="4" customWidth="1"/>
+    <col min="4359" max="4359" width="13" style="4" customWidth="1"/>
+    <col min="4360" max="4361" width="19.75" style="4" customWidth="1"/>
+    <col min="4362" max="4362" width="24.75" style="4" customWidth="1"/>
+    <col min="4363" max="4363" width="14.625" style="4" customWidth="1"/>
+    <col min="4364" max="4364" width="19.75" style="4" customWidth="1"/>
+    <col min="4365" max="4608" width="9" style="4"/>
+    <col min="4609" max="4609" width="11.5" style="4" customWidth="1"/>
+    <col min="4610" max="4610" width="21.375" style="4" customWidth="1"/>
+    <col min="4611" max="4611" width="18.625" style="4" customWidth="1"/>
+    <col min="4612" max="4612" width="23.125" style="4" customWidth="1"/>
+    <col min="4613" max="4613" width="20.875" style="4" customWidth="1"/>
+    <col min="4614" max="4614" width="21.125" style="4" customWidth="1"/>
+    <col min="4615" max="4615" width="13" style="4" customWidth="1"/>
+    <col min="4616" max="4617" width="19.75" style="4" customWidth="1"/>
+    <col min="4618" max="4618" width="24.75" style="4" customWidth="1"/>
+    <col min="4619" max="4619" width="14.625" style="4" customWidth="1"/>
+    <col min="4620" max="4620" width="19.75" style="4" customWidth="1"/>
+    <col min="4621" max="4864" width="9" style="4"/>
+    <col min="4865" max="4865" width="11.5" style="4" customWidth="1"/>
+    <col min="4866" max="4866" width="21.375" style="4" customWidth="1"/>
+    <col min="4867" max="4867" width="18.625" style="4" customWidth="1"/>
+    <col min="4868" max="4868" width="23.125" style="4" customWidth="1"/>
+    <col min="4869" max="4869" width="20.875" style="4" customWidth="1"/>
+    <col min="4870" max="4870" width="21.125" style="4" customWidth="1"/>
+    <col min="4871" max="4871" width="13" style="4" customWidth="1"/>
+    <col min="4872" max="4873" width="19.75" style="4" customWidth="1"/>
+    <col min="4874" max="4874" width="24.75" style="4" customWidth="1"/>
+    <col min="4875" max="4875" width="14.625" style="4" customWidth="1"/>
+    <col min="4876" max="4876" width="19.75" style="4" customWidth="1"/>
+    <col min="4877" max="5120" width="9" style="4"/>
+    <col min="5121" max="5121" width="11.5" style="4" customWidth="1"/>
+    <col min="5122" max="5122" width="21.375" style="4" customWidth="1"/>
+    <col min="5123" max="5123" width="18.625" style="4" customWidth="1"/>
+    <col min="5124" max="5124" width="23.125" style="4" customWidth="1"/>
+    <col min="5125" max="5125" width="20.875" style="4" customWidth="1"/>
+    <col min="5126" max="5126" width="21.125" style="4" customWidth="1"/>
+    <col min="5127" max="5127" width="13" style="4" customWidth="1"/>
+    <col min="5128" max="5129" width="19.75" style="4" customWidth="1"/>
+    <col min="5130" max="5130" width="24.75" style="4" customWidth="1"/>
+    <col min="5131" max="5131" width="14.625" style="4" customWidth="1"/>
+    <col min="5132" max="5132" width="19.75" style="4" customWidth="1"/>
+    <col min="5133" max="5376" width="9" style="4"/>
+    <col min="5377" max="5377" width="11.5" style="4" customWidth="1"/>
+    <col min="5378" max="5378" width="21.375" style="4" customWidth="1"/>
+    <col min="5379" max="5379" width="18.625" style="4" customWidth="1"/>
+    <col min="5380" max="5380" width="23.125" style="4" customWidth="1"/>
+    <col min="5381" max="5381" width="20.875" style="4" customWidth="1"/>
+    <col min="5382" max="5382" width="21.125" style="4" customWidth="1"/>
+    <col min="5383" max="5383" width="13" style="4" customWidth="1"/>
+    <col min="5384" max="5385" width="19.75" style="4" customWidth="1"/>
+    <col min="5386" max="5386" width="24.75" style="4" customWidth="1"/>
+    <col min="5387" max="5387" width="14.625" style="4" customWidth="1"/>
+    <col min="5388" max="5388" width="19.75" style="4" customWidth="1"/>
+    <col min="5389" max="5632" width="9" style="4"/>
+    <col min="5633" max="5633" width="11.5" style="4" customWidth="1"/>
+    <col min="5634" max="5634" width="21.375" style="4" customWidth="1"/>
+    <col min="5635" max="5635" width="18.625" style="4" customWidth="1"/>
+    <col min="5636" max="5636" width="23.125" style="4" customWidth="1"/>
+    <col min="5637" max="5637" width="20.875" style="4" customWidth="1"/>
+    <col min="5638" max="5638" width="21.125" style="4" customWidth="1"/>
+    <col min="5639" max="5639" width="13" style="4" customWidth="1"/>
+    <col min="5640" max="5641" width="19.75" style="4" customWidth="1"/>
+    <col min="5642" max="5642" width="24.75" style="4" customWidth="1"/>
+    <col min="5643" max="5643" width="14.625" style="4" customWidth="1"/>
+    <col min="5644" max="5644" width="19.75" style="4" customWidth="1"/>
+    <col min="5645" max="5888" width="9" style="4"/>
+    <col min="5889" max="5889" width="11.5" style="4" customWidth="1"/>
+    <col min="5890" max="5890" width="21.375" style="4" customWidth="1"/>
+    <col min="5891" max="5891" width="18.625" style="4" customWidth="1"/>
+    <col min="5892" max="5892" width="23.125" style="4" customWidth="1"/>
+    <col min="5893" max="5893" width="20.875" style="4" customWidth="1"/>
+    <col min="5894" max="5894" width="21.125" style="4" customWidth="1"/>
+    <col min="5895" max="5895" width="13" style="4" customWidth="1"/>
+    <col min="5896" max="5897" width="19.75" style="4" customWidth="1"/>
+    <col min="5898" max="5898" width="24.75" style="4" customWidth="1"/>
+    <col min="5899" max="5899" width="14.625" style="4" customWidth="1"/>
+    <col min="5900" max="5900" width="19.75" style="4" customWidth="1"/>
+    <col min="5901" max="6144" width="9" style="4"/>
+    <col min="6145" max="6145" width="11.5" style="4" customWidth="1"/>
+    <col min="6146" max="6146" width="21.375" style="4" customWidth="1"/>
+    <col min="6147" max="6147" width="18.625" style="4" customWidth="1"/>
+    <col min="6148" max="6148" width="23.125" style="4" customWidth="1"/>
+    <col min="6149" max="6149" width="20.875" style="4" customWidth="1"/>
+    <col min="6150" max="6150" width="21.125" style="4" customWidth="1"/>
+    <col min="6151" max="6151" width="13" style="4" customWidth="1"/>
+    <col min="6152" max="6153" width="19.75" style="4" customWidth="1"/>
+    <col min="6154" max="6154" width="24.75" style="4" customWidth="1"/>
+    <col min="6155" max="6155" width="14.625" style="4" customWidth="1"/>
+    <col min="6156" max="6156" width="19.75" style="4" customWidth="1"/>
+    <col min="6157" max="6400" width="9" style="4"/>
+    <col min="6401" max="6401" width="11.5" style="4" customWidth="1"/>
+    <col min="6402" max="6402" width="21.375" style="4" customWidth="1"/>
+    <col min="6403" max="6403" width="18.625" style="4" customWidth="1"/>
+    <col min="6404" max="6404" width="23.125" style="4" customWidth="1"/>
+    <col min="6405" max="6405" width="20.875" style="4" customWidth="1"/>
+    <col min="6406" max="6406" width="21.125" style="4" customWidth="1"/>
+    <col min="6407" max="6407" width="13" style="4" customWidth="1"/>
+    <col min="6408" max="6409" width="19.75" style="4" customWidth="1"/>
+    <col min="6410" max="6410" width="24.75" style="4" customWidth="1"/>
+    <col min="6411" max="6411" width="14.625" style="4" customWidth="1"/>
+    <col min="6412" max="6412" width="19.75" style="4" customWidth="1"/>
+    <col min="6413" max="6656" width="9" style="4"/>
+    <col min="6657" max="6657" width="11.5" style="4" customWidth="1"/>
+    <col min="6658" max="6658" width="21.375" style="4" customWidth="1"/>
+    <col min="6659" max="6659" width="18.625" style="4" customWidth="1"/>
+    <col min="6660" max="6660" width="23.125" style="4" customWidth="1"/>
+    <col min="6661" max="6661" width="20.875" style="4" customWidth="1"/>
+    <col min="6662" max="6662" width="21.125" style="4" customWidth="1"/>
+    <col min="6663" max="6663" width="13" style="4" customWidth="1"/>
+    <col min="6664" max="6665" width="19.75" style="4" customWidth="1"/>
+    <col min="6666" max="6666" width="24.75" style="4" customWidth="1"/>
+    <col min="6667" max="6667" width="14.625" style="4" customWidth="1"/>
+    <col min="6668" max="6668" width="19.75" style="4" customWidth="1"/>
+    <col min="6669" max="6912" width="9" style="4"/>
+    <col min="6913" max="6913" width="11.5" style="4" customWidth="1"/>
+    <col min="6914" max="6914" width="21.375" style="4" customWidth="1"/>
+    <col min="6915" max="6915" width="18.625" style="4" customWidth="1"/>
+    <col min="6916" max="6916" width="23.125" style="4" customWidth="1"/>
+    <col min="6917" max="6917" width="20.875" style="4" customWidth="1"/>
+    <col min="6918" max="6918" width="21.125" style="4" customWidth="1"/>
+    <col min="6919" max="6919" width="13" style="4" customWidth="1"/>
+    <col min="6920" max="6921" width="19.75" style="4" customWidth="1"/>
+    <col min="6922" max="6922" width="24.75" style="4" customWidth="1"/>
+    <col min="6923" max="6923" width="14.625" style="4" customWidth="1"/>
+    <col min="6924" max="6924" width="19.75" style="4" customWidth="1"/>
+    <col min="6925" max="7168" width="9" style="4"/>
+    <col min="7169" max="7169" width="11.5" style="4" customWidth="1"/>
+    <col min="7170" max="7170" width="21.375" style="4" customWidth="1"/>
+    <col min="7171" max="7171" width="18.625" style="4" customWidth="1"/>
+    <col min="7172" max="7172" width="23.125" style="4" customWidth="1"/>
+    <col min="7173" max="7173" width="20.875" style="4" customWidth="1"/>
+    <col min="7174" max="7174" width="21.125" style="4" customWidth="1"/>
+    <col min="7175" max="7175" width="13" style="4" customWidth="1"/>
+    <col min="7176" max="7177" width="19.75" style="4" customWidth="1"/>
+    <col min="7178" max="7178" width="24.75" style="4" customWidth="1"/>
+    <col min="7179" max="7179" width="14.625" style="4" customWidth="1"/>
+    <col min="7180" max="7180" width="19.75" style="4" customWidth="1"/>
+    <col min="7181" max="7424" width="9" style="4"/>
+    <col min="7425" max="7425" width="11.5" style="4" customWidth="1"/>
+    <col min="7426" max="7426" width="21.375" style="4" customWidth="1"/>
+    <col min="7427" max="7427" width="18.625" style="4" customWidth="1"/>
+    <col min="7428" max="7428" width="23.125" style="4" customWidth="1"/>
+    <col min="7429" max="7429" width="20.875" style="4" customWidth="1"/>
+    <col min="7430" max="7430" width="21.125" style="4" customWidth="1"/>
+    <col min="7431" max="7431" width="13" style="4" customWidth="1"/>
+    <col min="7432" max="7433" width="19.75" style="4" customWidth="1"/>
+    <col min="7434" max="7434" width="24.75" style="4" customWidth="1"/>
+    <col min="7435" max="7435" width="14.625" style="4" customWidth="1"/>
+    <col min="7436" max="7436" width="19.75" style="4" customWidth="1"/>
+    <col min="7437" max="7680" width="9" style="4"/>
+    <col min="7681" max="7681" width="11.5" style="4" customWidth="1"/>
+    <col min="7682" max="7682" width="21.375" style="4" customWidth="1"/>
+    <col min="7683" max="7683" width="18.625" style="4" customWidth="1"/>
+    <col min="7684" max="7684" width="23.125" style="4" customWidth="1"/>
+    <col min="7685" max="7685" width="20.875" style="4" customWidth="1"/>
+    <col min="7686" max="7686" width="21.125" style="4" customWidth="1"/>
+    <col min="7687" max="7687" width="13" style="4" customWidth="1"/>
+    <col min="7688" max="7689" width="19.75" style="4" customWidth="1"/>
+    <col min="7690" max="7690" width="24.75" style="4" customWidth="1"/>
+    <col min="7691" max="7691" width="14.625" style="4" customWidth="1"/>
+    <col min="7692" max="7692" width="19.75" style="4" customWidth="1"/>
+    <col min="7693" max="7936" width="9" style="4"/>
+    <col min="7937" max="7937" width="11.5" style="4" customWidth="1"/>
+    <col min="7938" max="7938" width="21.375" style="4" customWidth="1"/>
+    <col min="7939" max="7939" width="18.625" style="4" customWidth="1"/>
+    <col min="7940" max="7940" width="23.125" style="4" customWidth="1"/>
+    <col min="7941" max="7941" width="20.875" style="4" customWidth="1"/>
+    <col min="7942" max="7942" width="21.125" style="4" customWidth="1"/>
+    <col min="7943" max="7943" width="13" style="4" customWidth="1"/>
+    <col min="7944" max="7945" width="19.75" style="4" customWidth="1"/>
+    <col min="7946" max="7946" width="24.75" style="4" customWidth="1"/>
+    <col min="7947" max="7947" width="14.625" style="4" customWidth="1"/>
+    <col min="7948" max="7948" width="19.75" style="4" customWidth="1"/>
+    <col min="7949" max="8192" width="9" style="4"/>
+    <col min="8193" max="8193" width="11.5" style="4" customWidth="1"/>
+    <col min="8194" max="8194" width="21.375" style="4" customWidth="1"/>
+    <col min="8195" max="8195" width="18.625" style="4" customWidth="1"/>
+    <col min="8196" max="8196" width="23.125" style="4" customWidth="1"/>
+    <col min="8197" max="8197" width="20.875" style="4" customWidth="1"/>
+    <col min="8198" max="8198" width="21.125" style="4" customWidth="1"/>
+    <col min="8199" max="8199" width="13" style="4" customWidth="1"/>
+    <col min="8200" max="8201" width="19.75" style="4" customWidth="1"/>
+    <col min="8202" max="8202" width="24.75" style="4" customWidth="1"/>
+    <col min="8203" max="8203" width="14.625" style="4" customWidth="1"/>
+    <col min="8204" max="8204" width="19.75" style="4" customWidth="1"/>
+    <col min="8205" max="8448" width="9" style="4"/>
+    <col min="8449" max="8449" width="11.5" style="4" customWidth="1"/>
+    <col min="8450" max="8450" width="21.375" style="4" customWidth="1"/>
+    <col min="8451" max="8451" width="18.625" style="4" customWidth="1"/>
+    <col min="8452" max="8452" width="23.125" style="4" customWidth="1"/>
+    <col min="8453" max="8453" width="20.875" style="4" customWidth="1"/>
+    <col min="8454" max="8454" width="21.125" style="4" customWidth="1"/>
+    <col min="8455" max="8455" width="13" style="4" customWidth="1"/>
+    <col min="8456" max="8457" width="19.75" style="4" customWidth="1"/>
+    <col min="8458" max="8458" width="24.75" style="4" customWidth="1"/>
+    <col min="8459" max="8459" width="14.625" style="4" customWidth="1"/>
+    <col min="8460" max="8460" width="19.75" style="4" customWidth="1"/>
+    <col min="8461" max="8704" width="9" style="4"/>
+    <col min="8705" max="8705" width="11.5" style="4" customWidth="1"/>
+    <col min="8706" max="8706" width="21.375" style="4" customWidth="1"/>
+    <col min="8707" max="8707" width="18.625" style="4" customWidth="1"/>
+    <col min="8708" max="8708" width="23.125" style="4" customWidth="1"/>
+    <col min="8709" max="8709" width="20.875" style="4" customWidth="1"/>
+    <col min="8710" max="8710" width="21.125" style="4" customWidth="1"/>
+    <col min="8711" max="8711" width="13" style="4" customWidth="1"/>
+    <col min="8712" max="8713" width="19.75" style="4" customWidth="1"/>
+    <col min="8714" max="8714" width="24.75" style="4" customWidth="1"/>
+    <col min="8715" max="8715" width="14.625" style="4" customWidth="1"/>
+    <col min="8716" max="8716" width="19.75" style="4" customWidth="1"/>
+    <col min="8717" max="8960" width="9" style="4"/>
+    <col min="8961" max="8961" width="11.5" style="4" customWidth="1"/>
+    <col min="8962" max="8962" width="21.375" style="4" customWidth="1"/>
+    <col min="8963" max="8963" width="18.625" style="4" customWidth="1"/>
+    <col min="8964" max="8964" width="23.125" style="4" customWidth="1"/>
+    <col min="8965" max="8965" width="20.875" style="4" customWidth="1"/>
+    <col min="8966" max="8966" width="21.125" style="4" customWidth="1"/>
+    <col min="8967" max="8967" width="13" style="4" customWidth="1"/>
+    <col min="8968" max="8969" width="19.75" style="4" customWidth="1"/>
+    <col min="8970" max="8970" width="24.75" style="4" customWidth="1"/>
+    <col min="8971" max="8971" width="14.625" style="4" customWidth="1"/>
+    <col min="8972" max="8972" width="19.75" style="4" customWidth="1"/>
+    <col min="8973" max="9216" width="9" style="4"/>
+    <col min="9217" max="9217" width="11.5" style="4" customWidth="1"/>
+    <col min="9218" max="9218" width="21.375" style="4" customWidth="1"/>
+    <col min="9219" max="9219" width="18.625" style="4" customWidth="1"/>
+    <col min="9220" max="9220" width="23.125" style="4" customWidth="1"/>
+    <col min="9221" max="9221" width="20.875" style="4" customWidth="1"/>
+    <col min="9222" max="9222" width="21.125" style="4" customWidth="1"/>
+    <col min="9223" max="9223" width="13" style="4" customWidth="1"/>
+    <col min="9224" max="9225" width="19.75" style="4" customWidth="1"/>
+    <col min="9226" max="9226" width="24.75" style="4" customWidth="1"/>
+    <col min="9227" max="9227" width="14.625" style="4" customWidth="1"/>
+    <col min="9228" max="9228" width="19.75" style="4" customWidth="1"/>
+    <col min="9229" max="9472" width="9" style="4"/>
+    <col min="9473" max="9473" width="11.5" style="4" customWidth="1"/>
+    <col min="9474" max="9474" width="21.375" style="4" customWidth="1"/>
+    <col min="9475" max="9475" width="18.625" style="4" customWidth="1"/>
+    <col min="9476" max="9476" width="23.125" style="4" customWidth="1"/>
+    <col min="9477" max="9477" width="20.875" style="4" customWidth="1"/>
+    <col min="9478" max="9478" width="21.125" style="4" customWidth="1"/>
+    <col min="9479" max="9479" width="13" style="4" customWidth="1"/>
+    <col min="9480" max="9481" width="19.75" style="4" customWidth="1"/>
+    <col min="9482" max="9482" width="24.75" style="4" customWidth="1"/>
+    <col min="9483" max="9483" width="14.625" style="4" customWidth="1"/>
+    <col min="9484" max="9484" width="19.75" style="4" customWidth="1"/>
+    <col min="9485" max="9728" width="9" style="4"/>
+    <col min="9729" max="9729" width="11.5" style="4" customWidth="1"/>
+    <col min="9730" max="9730" width="21.375" style="4" customWidth="1"/>
+    <col min="9731" max="9731" width="18.625" style="4" customWidth="1"/>
+    <col min="9732" max="9732" width="23.125" style="4" customWidth="1"/>
+    <col min="9733" max="9733" width="20.875" style="4" customWidth="1"/>
+    <col min="9734" max="9734" width="21.125" style="4" customWidth="1"/>
+    <col min="9735" max="9735" width="13" style="4" customWidth="1"/>
+    <col min="9736" max="9737" width="19.75" style="4" customWidth="1"/>
+    <col min="9738" max="9738" width="24.75" style="4" customWidth="1"/>
+    <col min="9739" max="9739" width="14.625" style="4" customWidth="1"/>
+    <col min="9740" max="9740" width="19.75" style="4" customWidth="1"/>
+    <col min="9741" max="9984" width="9" style="4"/>
+    <col min="9985" max="9985" width="11.5" style="4" customWidth="1"/>
+    <col min="9986" max="9986" width="21.375" style="4" customWidth="1"/>
+    <col min="9987" max="9987" width="18.625" style="4" customWidth="1"/>
+    <col min="9988" max="9988" width="23.125" style="4" customWidth="1"/>
+    <col min="9989" max="9989" width="20.875" style="4" customWidth="1"/>
+    <col min="9990" max="9990" width="21.125" style="4" customWidth="1"/>
+    <col min="9991" max="9991" width="13" style="4" customWidth="1"/>
+    <col min="9992" max="9993" width="19.75" style="4" customWidth="1"/>
+    <col min="9994" max="9994" width="24.75" style="4" customWidth="1"/>
+    <col min="9995" max="9995" width="14.625" style="4" customWidth="1"/>
+    <col min="9996" max="9996" width="19.75" style="4" customWidth="1"/>
+    <col min="9997" max="10240" width="9" style="4"/>
+    <col min="10241" max="10241" width="11.5" style="4" customWidth="1"/>
+    <col min="10242" max="10242" width="21.375" style="4" customWidth="1"/>
+    <col min="10243" max="10243" width="18.625" style="4" customWidth="1"/>
+    <col min="10244" max="10244" width="23.125" style="4" customWidth="1"/>
+    <col min="10245" max="10245" width="20.875" style="4" customWidth="1"/>
+    <col min="10246" max="10246" width="21.125" style="4" customWidth="1"/>
+    <col min="10247" max="10247" width="13" style="4" customWidth="1"/>
+    <col min="10248" max="10249" width="19.75" style="4" customWidth="1"/>
+    <col min="10250" max="10250" width="24.75" style="4" customWidth="1"/>
+    <col min="10251" max="10251" width="14.625" style="4" customWidth="1"/>
+    <col min="10252" max="10252" width="19.75" style="4" customWidth="1"/>
+    <col min="10253" max="10496" width="9" style="4"/>
+    <col min="10497" max="10497" width="11.5" style="4" customWidth="1"/>
+    <col min="10498" max="10498" width="21.375" style="4" customWidth="1"/>
+    <col min="10499" max="10499" width="18.625" style="4" customWidth="1"/>
+    <col min="10500" max="10500" width="23.125" style="4" customWidth="1"/>
+    <col min="10501" max="10501" width="20.875" style="4" customWidth="1"/>
+    <col min="10502" max="10502" width="21.125" style="4" customWidth="1"/>
+    <col min="10503" max="10503" width="13" style="4" customWidth="1"/>
+    <col min="10504" max="10505" width="19.75" style="4" customWidth="1"/>
+    <col min="10506" max="10506" width="24.75" style="4" customWidth="1"/>
+    <col min="10507" max="10507" width="14.625" style="4" customWidth="1"/>
+    <col min="10508" max="10508" width="19.75" style="4" customWidth="1"/>
+    <col min="10509" max="10752" width="9" style="4"/>
+    <col min="10753" max="10753" width="11.5" style="4" customWidth="1"/>
+    <col min="10754" max="10754" width="21.375" style="4" customWidth="1"/>
+    <col min="10755" max="10755" width="18.625" style="4" customWidth="1"/>
+    <col min="10756" max="10756" width="23.125" style="4" customWidth="1"/>
+    <col min="10757" max="10757" width="20.875" style="4" customWidth="1"/>
+    <col min="10758" max="10758" width="21.125" style="4" customWidth="1"/>
+    <col min="10759" max="10759" width="13" style="4" customWidth="1"/>
+    <col min="10760" max="10761" width="19.75" style="4" customWidth="1"/>
+    <col min="10762" max="10762" width="24.75" style="4" customWidth="1"/>
+    <col min="10763" max="10763" width="14.625" style="4" customWidth="1"/>
+    <col min="10764" max="10764" width="19.75" style="4" customWidth="1"/>
+    <col min="10765" max="11008" width="9" style="4"/>
+    <col min="11009" max="11009" width="11.5" style="4" customWidth="1"/>
+    <col min="11010" max="11010" width="21.375" style="4" customWidth="1"/>
+    <col min="11011" max="11011" width="18.625" style="4" customWidth="1"/>
+    <col min="11012" max="11012" width="23.125" style="4" customWidth="1"/>
+    <col min="11013" max="11013" width="20.875" style="4" customWidth="1"/>
+    <col min="11014" max="11014" width="21.125" style="4" customWidth="1"/>
+    <col min="11015" max="11015" width="13" style="4" customWidth="1"/>
+    <col min="11016" max="11017" width="19.75" style="4" customWidth="1"/>
+    <col min="11018" max="11018" width="24.75" style="4" customWidth="1"/>
+    <col min="11019" max="11019" width="14.625" style="4" customWidth="1"/>
+    <col min="11020" max="11020" width="19.75" style="4" customWidth="1"/>
+    <col min="11021" max="11264" width="9" style="4"/>
+    <col min="11265" max="11265" width="11.5" style="4" customWidth="1"/>
+    <col min="11266" max="11266" width="21.375" style="4" customWidth="1"/>
+    <col min="11267" max="11267" width="18.625" style="4" customWidth="1"/>
+    <col min="11268" max="11268" width="23.125" style="4" customWidth="1"/>
+    <col min="11269" max="11269" width="20.875" style="4" customWidth="1"/>
+    <col min="11270" max="11270" width="21.125" style="4" customWidth="1"/>
+    <col min="11271" max="11271" width="13" style="4" customWidth="1"/>
+    <col min="11272" max="11273" width="19.75" style="4" customWidth="1"/>
+    <col min="11274" max="11274" width="24.75" style="4" customWidth="1"/>
+    <col min="11275" max="11275" width="14.625" style="4" customWidth="1"/>
+    <col min="11276" max="11276" width="19.75" style="4" customWidth="1"/>
+    <col min="11277" max="11520" width="9" style="4"/>
+    <col min="11521" max="11521" width="11.5" style="4" customWidth="1"/>
+    <col min="11522" max="11522" width="21.375" style="4" customWidth="1"/>
+    <col min="11523" max="11523" width="18.625" style="4" customWidth="1"/>
+    <col min="11524" max="11524" width="23.125" style="4" customWidth="1"/>
+    <col min="11525" max="11525" width="20.875" style="4" customWidth="1"/>
+    <col min="11526" max="11526" width="21.125" style="4" customWidth="1"/>
+    <col min="11527" max="11527" width="13" style="4" customWidth="1"/>
+    <col min="11528" max="11529" width="19.75" style="4" customWidth="1"/>
+    <col min="11530" max="11530" width="24.75" style="4" customWidth="1"/>
+    <col min="11531" max="11531" width="14.625" style="4" customWidth="1"/>
+    <col min="11532" max="11532" width="19.75" style="4" customWidth="1"/>
+    <col min="11533" max="11776" width="9" style="4"/>
+    <col min="11777" max="11777" width="11.5" style="4" customWidth="1"/>
+    <col min="11778" max="11778" width="21.375" style="4" customWidth="1"/>
+    <col min="11779" max="11779" width="18.625" style="4" customWidth="1"/>
+    <col min="11780" max="11780" width="23.125" style="4" customWidth="1"/>
+    <col min="11781" max="11781" width="20.875" style="4" customWidth="1"/>
+    <col min="11782" max="11782" width="21.125" style="4" customWidth="1"/>
+    <col min="11783" max="11783" width="13" style="4" customWidth="1"/>
+    <col min="11784" max="11785" width="19.75" style="4" customWidth="1"/>
+    <col min="11786" max="11786" width="24.75" style="4" customWidth="1"/>
+    <col min="11787" max="11787" width="14.625" style="4" customWidth="1"/>
+    <col min="11788" max="11788" width="19.75" style="4" customWidth="1"/>
+    <col min="11789" max="12032" width="9" style="4"/>
+    <col min="12033" max="12033" width="11.5" style="4" customWidth="1"/>
+    <col min="12034" max="12034" width="21.375" style="4" customWidth="1"/>
+    <col min="12035" max="12035" width="18.625" style="4" customWidth="1"/>
+    <col min="12036" max="12036" width="23.125" style="4" customWidth="1"/>
+    <col min="12037" max="12037" width="20.875" style="4" customWidth="1"/>
+    <col min="12038" max="12038" width="21.125" style="4" customWidth="1"/>
+    <col min="12039" max="12039" width="13" style="4" customWidth="1"/>
+    <col min="12040" max="12041" width="19.75" style="4" customWidth="1"/>
+    <col min="12042" max="12042" width="24.75" style="4" customWidth="1"/>
+    <col min="12043" max="12043" width="14.625" style="4" customWidth="1"/>
+    <col min="12044" max="12044" width="19.75" style="4" customWidth="1"/>
+    <col min="12045" max="12288" width="9" style="4"/>
+    <col min="12289" max="12289" width="11.5" style="4" customWidth="1"/>
+    <col min="12290" max="12290" width="21.375" style="4" customWidth="1"/>
+    <col min="12291" max="12291" width="18.625" style="4" customWidth="1"/>
+    <col min="12292" max="12292" width="23.125" style="4" customWidth="1"/>
+    <col min="12293" max="12293" width="20.875" style="4" customWidth="1"/>
+    <col min="12294" max="12294" width="21.125" style="4" customWidth="1"/>
+    <col min="12295" max="12295" width="13" style="4" customWidth="1"/>
+    <col min="12296" max="12297" width="19.75" style="4" customWidth="1"/>
+    <col min="12298" max="12298" width="24.75" style="4" customWidth="1"/>
+    <col min="12299" max="12299" width="14.625" style="4" customWidth="1"/>
+    <col min="12300" max="12300" width="19.75" style="4" customWidth="1"/>
+    <col min="12301" max="12544" width="9" style="4"/>
+    <col min="12545" max="12545" width="11.5" style="4" customWidth="1"/>
+    <col min="12546" max="12546" width="21.375" style="4" customWidth="1"/>
+    <col min="12547" max="12547" width="18.625" style="4" customWidth="1"/>
+    <col min="12548" max="12548" width="23.125" style="4" customWidth="1"/>
+    <col min="12549" max="12549" width="20.875" style="4" customWidth="1"/>
+    <col min="12550" max="12550" width="21.125" style="4" customWidth="1"/>
+    <col min="12551" max="12551" width="13" style="4" customWidth="1"/>
+    <col min="12552" max="12553" width="19.75" style="4" customWidth="1"/>
+    <col min="12554" max="12554" width="24.75" style="4" customWidth="1"/>
+    <col min="12555" max="12555" width="14.625" style="4" customWidth="1"/>
+    <col min="12556" max="12556" width="19.75" style="4" customWidth="1"/>
+    <col min="12557" max="12800" width="9" style="4"/>
+    <col min="12801" max="12801" width="11.5" style="4" customWidth="1"/>
+    <col min="12802" max="12802" width="21.375" style="4" customWidth="1"/>
+    <col min="12803" max="12803" width="18.625" style="4" customWidth="1"/>
+    <col min="12804" max="12804" width="23.125" style="4" customWidth="1"/>
+    <col min="12805" max="12805" width="20.875" style="4" customWidth="1"/>
+    <col min="12806" max="12806" width="21.125" style="4" customWidth="1"/>
+    <col min="12807" max="12807" width="13" style="4" customWidth="1"/>
+    <col min="12808" max="12809" width="19.75" style="4" customWidth="1"/>
+    <col min="12810" max="12810" width="24.75" style="4" customWidth="1"/>
+    <col min="12811" max="12811" width="14.625" style="4" customWidth="1"/>
+    <col min="12812" max="12812" width="19.75" style="4" customWidth="1"/>
+    <col min="12813" max="13056" width="9" style="4"/>
+    <col min="13057" max="13057" width="11.5" style="4" customWidth="1"/>
+    <col min="13058" max="13058" width="21.375" style="4" customWidth="1"/>
+    <col min="13059" max="13059" width="18.625" style="4" customWidth="1"/>
+    <col min="13060" max="13060" width="23.125" style="4" customWidth="1"/>
+    <col min="13061" max="13061" width="20.875" style="4" customWidth="1"/>
+    <col min="13062" max="13062" width="21.125" style="4" customWidth="1"/>
+    <col min="13063" max="13063" width="13" style="4" customWidth="1"/>
+    <col min="13064" max="13065" width="19.75" style="4" customWidth="1"/>
+    <col min="13066" max="13066" width="24.75" style="4" customWidth="1"/>
+    <col min="13067" max="13067" width="14.625" style="4" customWidth="1"/>
+    <col min="13068" max="13068" width="19.75" style="4" customWidth="1"/>
+    <col min="13069" max="13312" width="9" style="4"/>
+    <col min="13313" max="13313" width="11.5" style="4" customWidth="1"/>
+    <col min="13314" max="13314" width="21.375" style="4" customWidth="1"/>
+    <col min="13315" max="13315" width="18.625" style="4" customWidth="1"/>
+    <col min="13316" max="13316" width="23.125" style="4" customWidth="1"/>
+    <col min="13317" max="13317" width="20.875" style="4" customWidth="1"/>
+    <col min="13318" max="13318" width="21.125" style="4" customWidth="1"/>
+    <col min="13319" max="13319" width="13" style="4" customWidth="1"/>
+    <col min="13320" max="13321" width="19.75" style="4" customWidth="1"/>
+    <col min="13322" max="13322" width="24.75" style="4" customWidth="1"/>
+    <col min="13323" max="13323" width="14.625" style="4" customWidth="1"/>
+    <col min="13324" max="13324" width="19.75" style="4" customWidth="1"/>
+    <col min="13325" max="13568" width="9" style="4"/>
+    <col min="13569" max="13569" width="11.5" style="4" customWidth="1"/>
+    <col min="13570" max="13570" width="21.375" style="4" customWidth="1"/>
+    <col min="13571" max="13571" width="18.625" style="4" customWidth="1"/>
+    <col min="13572" max="13572" width="23.125" style="4" customWidth="1"/>
+    <col min="13573" max="13573" width="20.875" style="4" customWidth="1"/>
+    <col min="13574" max="13574" width="21.125" style="4" customWidth="1"/>
+    <col min="13575" max="13575" width="13" style="4" customWidth="1"/>
+    <col min="13576" max="13577" width="19.75" style="4" customWidth="1"/>
+    <col min="13578" max="13578" width="24.75" style="4" customWidth="1"/>
+    <col min="13579" max="13579" width="14.625" style="4" customWidth="1"/>
+    <col min="13580" max="13580" width="19.75" style="4" customWidth="1"/>
+    <col min="13581" max="13824" width="9" style="4"/>
+    <col min="13825" max="13825" width="11.5" style="4" customWidth="1"/>
+    <col min="13826" max="13826" width="21.375" style="4" customWidth="1"/>
+    <col min="13827" max="13827" width="18.625" style="4" customWidth="1"/>
+    <col min="13828" max="13828" width="23.125" style="4" customWidth="1"/>
+    <col min="13829" max="13829" width="20.875" style="4" customWidth="1"/>
+    <col min="13830" max="13830" width="21.125" style="4" customWidth="1"/>
+    <col min="13831" max="13831" width="13" style="4" customWidth="1"/>
+    <col min="13832" max="13833" width="19.75" style="4" customWidth="1"/>
+    <col min="13834" max="13834" width="24.75" style="4" customWidth="1"/>
+    <col min="13835" max="13835" width="14.625" style="4" customWidth="1"/>
+    <col min="13836" max="13836" width="19.75" style="4" customWidth="1"/>
+    <col min="13837" max="14080" width="9" style="4"/>
+    <col min="14081" max="14081" width="11.5" style="4" customWidth="1"/>
+    <col min="14082" max="14082" width="21.375" style="4" customWidth="1"/>
+    <col min="14083" max="14083" width="18.625" style="4" customWidth="1"/>
+    <col min="14084" max="14084" width="23.125" style="4" customWidth="1"/>
+    <col min="14085" max="14085" width="20.875" style="4" customWidth="1"/>
+    <col min="14086" max="14086" width="21.125" style="4" customWidth="1"/>
+    <col min="14087" max="14087" width="13" style="4" customWidth="1"/>
+    <col min="14088" max="14089" width="19.75" style="4" customWidth="1"/>
+    <col min="14090" max="14090" width="24.75" style="4" customWidth="1"/>
+    <col min="14091" max="14091" width="14.625" style="4" customWidth="1"/>
+    <col min="14092" max="14092" width="19.75" style="4" customWidth="1"/>
+    <col min="14093" max="14336" width="9" style="4"/>
+    <col min="14337" max="14337" width="11.5" style="4" customWidth="1"/>
+    <col min="14338" max="14338" width="21.375" style="4" customWidth="1"/>
+    <col min="14339" max="14339" width="18.625" style="4" customWidth="1"/>
+    <col min="14340" max="14340" width="23.125" style="4" customWidth="1"/>
+    <col min="14341" max="14341" width="20.875" style="4" customWidth="1"/>
+    <col min="14342" max="14342" width="21.125" style="4" customWidth="1"/>
+    <col min="14343" max="14343" width="13" style="4" customWidth="1"/>
+    <col min="14344" max="14345" width="19.75" style="4" customWidth="1"/>
+    <col min="14346" max="14346" width="24.75" style="4" customWidth="1"/>
+    <col min="14347" max="14347" width="14.625" style="4" customWidth="1"/>
+    <col min="14348" max="14348" width="19.75" style="4" customWidth="1"/>
+    <col min="14349" max="14592" width="9" style="4"/>
+    <col min="14593" max="14593" width="11.5" style="4" customWidth="1"/>
+    <col min="14594" max="14594" width="21.375" style="4" customWidth="1"/>
+    <col min="14595" max="14595" width="18.625" style="4" customWidth="1"/>
+    <col min="14596" max="14596" width="23.125" style="4" customWidth="1"/>
+    <col min="14597" max="14597" width="20.875" style="4" customWidth="1"/>
+    <col min="14598" max="14598" width="21.125" style="4" customWidth="1"/>
+    <col min="14599" max="14599" width="13" style="4" customWidth="1"/>
+    <col min="14600" max="14601" width="19.75" style="4" customWidth="1"/>
+    <col min="14602" max="14602" width="24.75" style="4" customWidth="1"/>
+    <col min="14603" max="14603" width="14.625" style="4" customWidth="1"/>
+    <col min="14604" max="14604" width="19.75" style="4" customWidth="1"/>
+    <col min="14605" max="14848" width="9" style="4"/>
+    <col min="14849" max="14849" width="11.5" style="4" customWidth="1"/>
+    <col min="14850" max="14850" width="21.375" style="4" customWidth="1"/>
+    <col min="14851" max="14851" width="18.625" style="4" customWidth="1"/>
+    <col min="14852" max="14852" width="23.125" style="4" customWidth="1"/>
+    <col min="14853" max="14853" width="20.875" style="4" customWidth="1"/>
+    <col min="14854" max="14854" width="21.125" style="4" customWidth="1"/>
+    <col min="14855" max="14855" width="13" style="4" customWidth="1"/>
+    <col min="14856" max="14857" width="19.75" style="4" customWidth="1"/>
+    <col min="14858" max="14858" width="24.75" style="4" customWidth="1"/>
+    <col min="14859" max="14859" width="14.625" style="4" customWidth="1"/>
+    <col min="14860" max="14860" width="19.75" style="4" customWidth="1"/>
+    <col min="14861" max="15104" width="9" style="4"/>
+    <col min="15105" max="15105" width="11.5" style="4" customWidth="1"/>
+    <col min="15106" max="15106" width="21.375" style="4" customWidth="1"/>
+    <col min="15107" max="15107" width="18.625" style="4" customWidth="1"/>
+    <col min="15108" max="15108" width="23.125" style="4" customWidth="1"/>
+    <col min="15109" max="15109" width="20.875" style="4" customWidth="1"/>
+    <col min="15110" max="15110" width="21.125" style="4" customWidth="1"/>
+    <col min="15111" max="15111" width="13" style="4" customWidth="1"/>
+    <col min="15112" max="15113" width="19.75" style="4" customWidth="1"/>
+    <col min="15114" max="15114" width="24.75" style="4" customWidth="1"/>
+    <col min="15115" max="15115" width="14.625" style="4" customWidth="1"/>
+    <col min="15116" max="15116" width="19.75" style="4" customWidth="1"/>
+    <col min="15117" max="15360" width="9" style="4"/>
+    <col min="15361" max="15361" width="11.5" style="4" customWidth="1"/>
+    <col min="15362" max="15362" width="21.375" style="4" customWidth="1"/>
+    <col min="15363" max="15363" width="18.625" style="4" customWidth="1"/>
+    <col min="15364" max="15364" width="23.125" style="4" customWidth="1"/>
+    <col min="15365" max="15365" width="20.875" style="4" customWidth="1"/>
+    <col min="15366" max="15366" width="21.125" style="4" customWidth="1"/>
+    <col min="15367" max="15367" width="13" style="4" customWidth="1"/>
+    <col min="15368" max="15369" width="19.75" style="4" customWidth="1"/>
+    <col min="15370" max="15370" width="24.75" style="4" customWidth="1"/>
+    <col min="15371" max="15371" width="14.625" style="4" customWidth="1"/>
+    <col min="15372" max="15372" width="19.75" style="4" customWidth="1"/>
+    <col min="15373" max="15616" width="9" style="4"/>
+    <col min="15617" max="15617" width="11.5" style="4" customWidth="1"/>
+    <col min="15618" max="15618" width="21.375" style="4" customWidth="1"/>
+    <col min="15619" max="15619" width="18.625" style="4" customWidth="1"/>
+    <col min="15620" max="15620" width="23.125" style="4" customWidth="1"/>
+    <col min="15621" max="15621" width="20.875" style="4" customWidth="1"/>
+    <col min="15622" max="15622" width="21.125" style="4" customWidth="1"/>
+    <col min="15623" max="15623" width="13" style="4" customWidth="1"/>
+    <col min="15624" max="15625" width="19.75" style="4" customWidth="1"/>
+    <col min="15626" max="15626" width="24.75" style="4" customWidth="1"/>
+    <col min="15627" max="15627" width="14.625" style="4" customWidth="1"/>
+    <col min="15628" max="15628" width="19.75" style="4" customWidth="1"/>
+    <col min="15629" max="15872" width="9" style="4"/>
+    <col min="15873" max="15873" width="11.5" style="4" customWidth="1"/>
+    <col min="15874" max="15874" width="21.375" style="4" customWidth="1"/>
+    <col min="15875" max="15875" width="18.625" style="4" customWidth="1"/>
+    <col min="15876" max="15876" width="23.125" style="4" customWidth="1"/>
+    <col min="15877" max="15877" width="20.875" style="4" customWidth="1"/>
+    <col min="15878" max="15878" width="21.125" style="4" customWidth="1"/>
+    <col min="15879" max="15879" width="13" style="4" customWidth="1"/>
+    <col min="15880" max="15881" width="19.75" style="4" customWidth="1"/>
+    <col min="15882" max="15882" width="24.75" style="4" customWidth="1"/>
+    <col min="15883" max="15883" width="14.625" style="4" customWidth="1"/>
+    <col min="15884" max="15884" width="19.75" style="4" customWidth="1"/>
+    <col min="15885" max="16128" width="9" style="4"/>
+    <col min="16129" max="16129" width="11.5" style="4" customWidth="1"/>
+    <col min="16130" max="16130" width="21.375" style="4" customWidth="1"/>
+    <col min="16131" max="16131" width="18.625" style="4" customWidth="1"/>
+    <col min="16132" max="16132" width="23.125" style="4" customWidth="1"/>
+    <col min="16133" max="16133" width="20.875" style="4" customWidth="1"/>
+    <col min="16134" max="16134" width="21.125" style="4" customWidth="1"/>
+    <col min="16135" max="16135" width="13" style="4" customWidth="1"/>
+    <col min="16136" max="16137" width="19.75" style="4" customWidth="1"/>
+    <col min="16138" max="16138" width="24.75" style="4" customWidth="1"/>
+    <col min="16139" max="16139" width="14.625" style="4" customWidth="1"/>
+    <col min="16140" max="16140" width="19.75" style="4" customWidth="1"/>
+    <col min="16141" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
     <row r="1" ht="24.75" customHeight="1" spans="1:9">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="9" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
     </row>
     <row r="2" ht="15" spans="1:13">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="32" t="s">
+      <c r="L2" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="10"/>
+      <c r="M2" s="7"/>
     </row>
     <row r="3" ht="15" spans="1:13">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="10"/>
+      <c r="M3" s="7"/>
     </row>
     <row r="4" ht="15" spans="1:13">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="13" t="s">
+      <c r="K4" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="19" t="s">
+      <c r="L4" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="10"/>
+      <c r="M4" s="7"/>
     </row>
     <row r="5" ht="15" spans="1:13">
-      <c r="A5" s="14">
+      <c r="A5" s="11">
         <v>1024</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="11">
         <v>3</v>
       </c>
-      <c r="K5" s="14">
+      <c r="K5" s="11">
         <v>2</v>
       </c>
-      <c r="L5" s="23">
+      <c r="L5" s="20">
         <v>42201.8370138889</v>
       </c>
-      <c r="M5" s="10"/>
+      <c r="M5" s="7"/>
     </row>
     <row r="6" ht="15" spans="1:13">
-      <c r="A6" s="14">
+      <c r="A6" s="11">
         <v>1025</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="11">
         <v>2</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="I6" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="11">
         <v>2</v>
       </c>
-      <c r="K6" s="14">
+      <c r="K6" s="11">
         <v>1</v>
       </c>
-      <c r="L6" s="23">
+      <c r="L6" s="20">
         <v>42202.0036805556</v>
       </c>
-      <c r="M6" s="10"/>
+      <c r="M6" s="7"/>
     </row>
     <row r="7" ht="15" spans="1:13">
-      <c r="A7" s="14">
+      <c r="A7" s="11">
         <v>1026</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="11">
         <v>1</v>
       </c>
-      <c r="K7" s="14">
+      <c r="K7" s="11">
         <v>3</v>
       </c>
-      <c r="L7" s="23">
+      <c r="L7" s="20">
         <v>42203.4203472222</v>
       </c>
-      <c r="M7" s="10"/>
+      <c r="M7" s="7"/>
     </row>
     <row r="8" ht="15" spans="1:9">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="10"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="7"/>
     </row>
     <row r="9" ht="15" spans="1:9">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="9" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
     </row>
     <row r="10" ht="15" spans="1:14">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="32" t="s">
+      <c r="F10" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="G10" s="32" t="s">
+      <c r="G10" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="32" t="s">
+      <c r="H10" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="I10" s="32" t="s">
+      <c r="I10" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="32" t="s">
+      <c r="J10" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="K10" s="32" t="s">
+      <c r="K10" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="L10" s="32" t="s">
+      <c r="L10" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="M10" s="32" t="s">
+      <c r="M10" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="N10" s="10"/>
+      <c r="N10" s="7"/>
     </row>
     <row r="11" ht="15" spans="1:14">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="H11" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="I11" s="12" t="s">
+      <c r="I11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="J11" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="K11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="L11" s="12" t="s">
+      <c r="L11" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="M11" s="12" t="s">
+      <c r="M11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="N11" s="10"/>
+      <c r="N11" s="7"/>
     </row>
     <row r="12" ht="15" spans="1:14">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="J12" s="13" t="s">
+      <c r="J12" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="K12" s="13" t="s">
+      <c r="K12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="L12" s="13" t="s">
+      <c r="L12" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="M12" s="19" t="s">
+      <c r="M12" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="N12" s="10"/>
+      <c r="N12" s="7"/>
     </row>
     <row r="13" ht="15" spans="1:14">
-      <c r="A13" s="14">
+      <c r="A13" s="11">
         <v>2001</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="11">
         <v>1</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="G13" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="I13" s="14" t="s">
+      <c r="I13" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="J13" s="14" t="s">
+      <c r="J13" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="K13" s="14" t="s">
+      <c r="K13" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="L13" s="14" t="s">
+      <c r="L13" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="M13" s="23">
+      <c r="M13" s="20">
         <v>42201.8370138889</v>
       </c>
-      <c r="N13" s="10"/>
+      <c r="N13" s="7"/>
     </row>
     <row r="14" ht="15" spans="1:14">
-      <c r="A14" s="14">
+      <c r="A14" s="11">
         <v>2002</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="11">
         <v>5</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="G14" s="22" t="s">
+      <c r="G14" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="J14" s="14" t="s">
+      <c r="J14" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="K14" s="14" t="s">
+      <c r="K14" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="L14" s="14" t="s">
+      <c r="L14" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="M14" s="23">
+      <c r="M14" s="20">
         <v>42202.0036805556</v>
       </c>
-      <c r="N14" s="10"/>
+      <c r="N14" s="7"/>
     </row>
     <row r="15" ht="15" spans="1:14">
-      <c r="A15" s="14">
+      <c r="A15" s="11">
         <v>2003</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="11">
         <v>2</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="G15" s="22" t="s">
+      <c r="G15" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="H15" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="I15" s="14" t="s">
+      <c r="I15" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="J15" s="14" t="s">
+      <c r="J15" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="K15" s="14" t="s">
+      <c r="K15" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="L15" s="14" t="s">
+      <c r="L15" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="M15" s="23">
+      <c r="M15" s="20">
         <v>42203.4203472222</v>
       </c>
-      <c r="N15" s="10"/>
+      <c r="N15" s="7"/>
     </row>
     <row r="16" ht="15" spans="1:9">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="10"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="7"/>
     </row>
     <row r="17" ht="23.25" customHeight="1" spans="1:9">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="16" t="s">
+      <c r="B17" s="5"/>
+      <c r="C17" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
     </row>
     <row r="18" ht="15" spans="1:13">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="32" t="s">
+      <c r="D18" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="32" t="s">
+      <c r="F18" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="G18" s="32" t="s">
+      <c r="G18" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="H18" s="32" t="s">
+      <c r="H18" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="I18" s="32" t="s">
+      <c r="I18" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="J18" s="32" t="s">
+      <c r="J18" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
     </row>
     <row r="19" ht="15" spans="1:13">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F19" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="G19" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="12" t="s">
+      <c r="H19" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="I19" s="12" t="s">
+      <c r="I19" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="J19" s="12" t="s">
+      <c r="J19" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
     </row>
     <row r="20" ht="15" spans="1:13">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="19" t="s">
+      <c r="F20" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="H20" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="I20" s="13" t="s">
+      <c r="I20" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="J20" s="13" t="s">
+      <c r="J20" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
     </row>
     <row r="21" ht="15" spans="1:13">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C21" s="14">
+      <c r="C21" s="11">
         <v>1</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="E21" s="22">
+      <c r="E21" s="19">
         <v>1</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G21" s="11">
         <v>1</v>
       </c>
-      <c r="H21" s="7" t="s">
+      <c r="H21" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="I21" s="14">
+      <c r="I21" s="11">
         <v>1</v>
       </c>
-      <c r="J21" s="7" t="s">
+      <c r="J21" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
     </row>
     <row r="22" ht="15" spans="1:13">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C22" s="14">
+      <c r="C22" s="11">
         <v>2</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E22" s="22">
+      <c r="E22" s="19">
         <v>2</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="G22" s="14">
+      <c r="G22" s="11">
         <v>2</v>
       </c>
-      <c r="H22" s="7" t="s">
+      <c r="H22" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="I22" s="14">
+      <c r="I22" s="11">
         <v>2</v>
       </c>
-      <c r="J22" s="7" t="s">
+      <c r="J22" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
     </row>
     <row r="23" ht="15" spans="1:13">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="11">
         <v>3</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="E23" s="22">
+      <c r="E23" s="19">
         <v>3</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="G23" s="14">
+      <c r="G23" s="11">
         <v>3</v>
       </c>
-      <c r="H23" s="7" t="s">
+      <c r="H23" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="I23" s="14">
+      <c r="I23" s="11">
         <v>3</v>
       </c>
-      <c r="J23" s="7" t="s">
+      <c r="J23" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
     </row>
     <row r="24" ht="15" spans="1:13">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11">
         <v>4</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="E24" s="22">
+      <c r="E24" s="19">
         <v>4</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="G24" s="22">
+      <c r="G24" s="19">
         <v>4</v>
       </c>
-      <c r="H24" s="7" t="s">
+      <c r="H24" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="I24" s="22">
+      <c r="I24" s="19">
         <v>4</v>
       </c>
-      <c r="J24" s="7" t="s">
+      <c r="J24" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
     </row>
     <row r="25" ht="15" spans="1:13">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11">
         <v>5</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="E25" s="22">
+      <c r="E25" s="19">
         <v>5</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="G25" s="22">
+      <c r="G25" s="19">
         <v>5</v>
       </c>
-      <c r="H25" s="7" t="s">
+      <c r="H25" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="I25" s="22">
+      <c r="I25" s="19">
         <v>5</v>
       </c>
-      <c r="J25" s="7" t="s">
+      <c r="J25" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
     </row>
     <row r="26" ht="15" spans="1:13">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14">
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11">
         <v>6</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="E26" s="22">
+      <c r="E26" s="19">
         <v>6</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="G26" s="22">
+      <c r="G26" s="19">
         <v>6</v>
       </c>
-      <c r="H26" s="7" t="s">
+      <c r="H26" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="I26" s="22">
+      <c r="I26" s="19">
         <v>6</v>
       </c>
-      <c r="J26" s="7" t="s">
+      <c r="J26" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
     </row>
     <row r="27" ht="15" spans="1:13">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14">
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11">
         <v>7</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E27" s="22">
+      <c r="E27" s="19">
         <v>7</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G27" s="22">
+      <c r="G27" s="19">
         <v>7</v>
       </c>
-      <c r="H27" s="7" t="s">
+      <c r="H27" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="I27" s="22">
+      <c r="I27" s="19">
         <v>7</v>
       </c>
-      <c r="J27" s="7" t="s">
+      <c r="J27" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
     </row>
     <row r="28" ht="15" spans="1:13">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14">
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11">
         <v>8</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="E28" s="22">
+      <c r="E28" s="19">
         <v>8</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="G28" s="22">
+      <c r="G28" s="19">
         <v>8</v>
       </c>
-      <c r="H28" s="7" t="s">
+      <c r="H28" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="I28" s="22">
+      <c r="I28" s="19">
         <v>8</v>
       </c>
-      <c r="J28" s="7" t="s">
+      <c r="J28" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
     </row>
     <row r="29" ht="15" spans="1:10">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="22">
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="19">
         <v>9</v>
       </c>
-      <c r="F29" s="26" t="s">
+      <c r="F29" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="G29" s="22">
+      <c r="G29" s="19">
         <v>9</v>
       </c>
-      <c r="H29" s="7" t="s">
+      <c r="H29" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="I29" s="22">
+      <c r="I29" s="19">
         <v>9</v>
       </c>
-      <c r="J29" s="7" t="s">
+      <c r="J29" s="4" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="30" ht="15" spans="1:10">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="22"/>
-      <c r="G30" s="22">
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="19"/>
+      <c r="G30" s="19">
         <v>10</v>
       </c>
-      <c r="H30" s="7" t="s">
+      <c r="H30" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="I30" s="22">
+      <c r="I30" s="19">
         <v>10</v>
       </c>
-      <c r="J30" s="7" t="s">
+      <c r="J30" s="4" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="31" ht="15" spans="1:10">
-      <c r="A31" s="14"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="22"/>
-      <c r="G31" s="22">
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="19"/>
+      <c r="G31" s="19">
         <v>11</v>
       </c>
-      <c r="H31" s="7" t="s">
+      <c r="H31" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="I31" s="22">
+      <c r="I31" s="19">
         <v>11</v>
       </c>
-      <c r="J31" s="7" t="s">
+      <c r="J31" s="4" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="32" ht="15" spans="1:10">
-      <c r="A32" s="14"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="I32" s="22">
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="I32" s="19">
         <v>12</v>
       </c>
-      <c r="J32" s="7" t="s">
+      <c r="J32" s="4" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="33" ht="15" spans="1:10">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="22"/>
-      <c r="G33" s="22"/>
-      <c r="I33" s="22">
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="I33" s="19">
         <v>13</v>
       </c>
-      <c r="J33" s="7" t="s">
+      <c r="J33" s="4" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="34" ht="15" spans="1:9">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="16" t="s">
+      <c r="B34" s="5"/>
+      <c r="C34" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="D34" s="14"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="23"/>
-      <c r="I34" s="10"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="7"/>
     </row>
     <row r="35" ht="15" spans="1:8">
-      <c r="A35" s="32" t="s">
+      <c r="A35" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="B35" s="32" t="s">
+      <c r="B35" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="C35" s="32" t="s">
+      <c r="C35" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="D35" s="32" t="s">
+      <c r="D35" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="E35" s="32" t="s">
+      <c r="E35" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="F35" s="32" t="s">
+      <c r="F35" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="G35" s="32" t="s">
+      <c r="G35" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="H35" s="10"/>
+      <c r="H35" s="7"/>
     </row>
     <row r="36" ht="15" spans="1:8">
-      <c r="A36" s="12" t="s">
+      <c r="A36" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="D36" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="E36" s="12" t="s">
+      <c r="E36" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="F36" s="12" t="s">
+      <c r="F36" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G36" s="12" t="s">
+      <c r="G36" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H36" s="10"/>
+      <c r="H36" s="7"/>
     </row>
     <row r="37" ht="15" spans="1:8">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="D37" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="E37" s="13" t="s">
+      <c r="E37" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="F37" s="13" t="s">
+      <c r="F37" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="G37" s="19" t="s">
+      <c r="G37" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="H37" s="10"/>
+      <c r="H37" s="7"/>
     </row>
     <row r="38" ht="15" spans="1:9">
-      <c r="A38" s="17"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="10"/>
+      <c r="A38" s="14"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="7"/>
     </row>
     <row r="39" ht="15" spans="1:8">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="16" t="s">
+      <c r="B39" s="6"/>
+      <c r="C39" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
     </row>
     <row r="40" ht="15" spans="1:8">
-      <c r="A40" s="32" t="s">
+      <c r="A40" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="B40" s="32" t="s">
+      <c r="B40" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C40" s="32" t="s">
+      <c r="C40" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="D40" s="32" t="s">
+      <c r="D40" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
     </row>
     <row r="41" ht="15" spans="1:8">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="C41" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D41" s="12" t="s">
+      <c r="D41" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
     </row>
     <row r="42" ht="15" spans="1:8">
-      <c r="A42" s="18"/>
-      <c r="B42" s="19" t="s">
+      <c r="A42" s="15"/>
+      <c r="B42" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="19" t="s">
+      <c r="C42" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D42" s="19" t="s">
+      <c r="D42" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
     </row>
     <row r="43" ht="15" spans="1:8">
-      <c r="A43" s="10"/>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="10"/>
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
     </row>
     <row r="44" ht="15" spans="1:4">
-      <c r="A44" s="9" t="s">
+      <c r="A44" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="B44" s="9"/>
-      <c r="C44" s="16" t="s">
+      <c r="B44" s="6"/>
+      <c r="C44" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="D44" s="10"/>
+      <c r="D44" s="7"/>
     </row>
     <row r="45" ht="14.25" customHeight="1" spans="1:7">
-      <c r="A45" s="32" t="s">
+      <c r="A45" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B45" s="32" t="s">
+      <c r="B45" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="C45" s="32" t="s">
+      <c r="C45" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="D45" s="32" t="s">
+      <c r="D45" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="E45" s="32" t="s">
+      <c r="E45" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="F45" s="27" t="s">
+      <c r="F45" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="G45" s="28"/>
+      <c r="G45" s="25"/>
     </row>
     <row r="46" ht="14.25" customHeight="1" spans="1:7">
-      <c r="A46" s="12" t="s">
+      <c r="A46" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="12" t="s">
+      <c r="B46" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C46" s="12" t="s">
+      <c r="C46" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D46" s="12" t="s">
+      <c r="D46" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="E46" s="12" t="s">
+      <c r="E46" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="F46" s="27"/>
-      <c r="G46" s="28"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="25"/>
     </row>
     <row r="47" ht="14.25" customHeight="1" spans="1:7">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B47" s="13" t="s">
+      <c r="B47" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C47" s="19" t="s">
+      <c r="C47" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D47" s="19" t="s">
+      <c r="D47" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="E47" s="19" t="s">
+      <c r="E47" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="F47" s="27"/>
-      <c r="G47" s="28"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" ht="14.25" customHeight="1" spans="1:7">
-      <c r="A48" s="14">
+      <c r="A48" s="11">
         <v>1024</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C48" s="14">
+      <c r="C48" s="11">
         <v>2001</v>
       </c>
-      <c r="D48" s="20">
+      <c r="D48" s="17">
         <v>1</v>
       </c>
-      <c r="E48" s="29">
+      <c r="E48" s="26">
         <v>0.5612</v>
       </c>
-      <c r="F48" s="30" t="s">
+      <c r="F48" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="G48" s="30"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" ht="15" spans="3:7">
-      <c r="C49" s="14">
+      <c r="C49" s="11">
         <v>2002</v>
       </c>
-      <c r="D49" s="21">
+      <c r="D49" s="18">
         <v>2</v>
       </c>
-      <c r="E49" s="31">
+      <c r="E49" s="28">
         <v>0.6343</v>
       </c>
-      <c r="F49" s="30"/>
-      <c r="G49" s="30"/>
+      <c r="F49" s="27"/>
+      <c r="G49" s="27"/>
     </row>
     <row r="50" ht="15" spans="3:7">
-      <c r="C50" s="14">
+      <c r="C50" s="11">
         <v>2003</v>
       </c>
-      <c r="D50" s="21">
+      <c r="D50" s="18">
         <v>3</v>
       </c>
-      <c r="E50" s="31">
+      <c r="E50" s="28">
         <v>0.1274</v>
       </c>
-      <c r="F50" s="30"/>
-      <c r="G50" s="30"/>
+      <c r="F50" s="27"/>
+      <c r="G50" s="27"/>
     </row>
     <row r="51" ht="15" spans="1:7">
-      <c r="A51" s="14">
+      <c r="A51" s="11">
         <v>1025</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B51" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C51" s="14">
+      <c r="C51" s="11">
         <v>2001</v>
       </c>
-      <c r="D51" s="21">
+      <c r="D51" s="18">
         <v>2</v>
       </c>
-      <c r="E51" s="29">
+      <c r="E51" s="26">
         <v>0.8532</v>
       </c>
-      <c r="F51" s="30"/>
-      <c r="G51" s="30"/>
+      <c r="F51" s="27"/>
+      <c r="G51" s="27"/>
     </row>
     <row r="52" ht="15" spans="3:7">
-      <c r="C52" s="14">
+      <c r="C52" s="11">
         <v>2002</v>
       </c>
-      <c r="D52" s="21">
+      <c r="D52" s="18">
         <v>1</v>
       </c>
-      <c r="E52" s="31">
+      <c r="E52" s="28">
         <v>0.1243</v>
       </c>
-      <c r="F52" s="30"/>
-      <c r="G52" s="30"/>
+      <c r="F52" s="27"/>
+      <c r="G52" s="27"/>
     </row>
     <row r="53" ht="15" spans="3:7">
-      <c r="C53" s="14">
+      <c r="C53" s="11">
         <v>2003</v>
       </c>
-      <c r="D53" s="21">
+      <c r="D53" s="18">
         <v>3</v>
       </c>
-      <c r="E53" s="31">
+      <c r="E53" s="28">
         <v>0.5231</v>
       </c>
-      <c r="F53" s="30"/>
-      <c r="G53" s="30"/>
+      <c r="F53" s="27"/>
+      <c r="G53" s="27"/>
     </row>
     <row r="54" ht="15" spans="1:7">
-      <c r="A54" s="14">
+      <c r="A54" s="11">
         <v>1026</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C54" s="14">
+      <c r="C54" s="11">
         <v>2001</v>
       </c>
-      <c r="D54" s="21">
+      <c r="D54" s="18">
         <v>3</v>
       </c>
-      <c r="E54" s="29">
+      <c r="E54" s="26">
         <v>0.6835</v>
       </c>
-      <c r="F54" s="30"/>
-      <c r="G54" s="30"/>
+      <c r="F54" s="27"/>
+      <c r="G54" s="27"/>
     </row>
     <row r="55" ht="15" spans="3:7">
-      <c r="C55" s="14">
+      <c r="C55" s="11">
         <v>2002</v>
       </c>
-      <c r="D55" s="21">
+      <c r="D55" s="18">
         <v>1</v>
       </c>
-      <c r="E55" s="31">
+      <c r="E55" s="28">
         <v>0.1208</v>
       </c>
-      <c r="F55" s="30"/>
-      <c r="G55" s="30"/>
+      <c r="F55" s="27"/>
+      <c r="G55" s="27"/>
     </row>
     <row r="56" ht="15" spans="3:7">
-      <c r="C56" s="14">
+      <c r="C56" s="11">
         <v>2003</v>
       </c>
-      <c r="D56" s="21">
+      <c r="D56" s="18">
         <v>2</v>
       </c>
-      <c r="E56" s="31">
+      <c r="E56" s="28">
         <v>0.5742</v>
       </c>
-      <c r="F56" s="30"/>
-      <c r="G56" s="30"/>
+      <c r="F56" s="27"/>
+      <c r="G56" s="27"/>
     </row>
     <row r="57" spans="6:7">
-      <c r="F57" s="30"/>
-      <c r="G57" s="30"/>
+      <c r="F57" s="27"/>
+      <c r="G57" s="27"/>
     </row>
     <row r="58" spans="6:7">
-      <c r="F58" s="30"/>
-      <c r="G58" s="30"/>
+      <c r="F58" s="27"/>
+      <c r="G58" s="27"/>
     </row>
     <row r="59" spans="6:7">
-      <c r="F59" s="30"/>
-      <c r="G59" s="30"/>
+      <c r="F59" s="27"/>
+      <c r="G59" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3758,7 +3748,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -3801,7 +3791,7 @@
       <c r="K1" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="2" t="s">
         <v>179</v>
       </c>
     </row>
@@ -3815,27 +3805,27 @@
       <c r="C2" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>181</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>181</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="2" t="s">
         <v>181</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="J2" s="4"/>
+      <c r="J2" s="2"/>
       <c r="K2" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="2" t="s">
         <v>181</v>
       </c>
     </row>
@@ -3867,37 +3857,37 @@
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="5"/>
+      <c r="L3" s="2"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>181</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>181</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="2" t="s">
         <v>181</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="2" t="s">
         <v>181</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="J4" s="4"/>
+      <c r="J4" s="2"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="5"/>
+      <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
@@ -3927,41 +3917,41 @@
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="5"/>
+      <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>181</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="2" t="s">
         <v>181</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="2" t="s">
         <v>181</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="2" t="s">
         <v>181</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="2" t="s">
         <v>181</v>
       </c>
       <c r="K6" s="1"/>
-      <c r="L6" s="5"/>
+      <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
@@ -3981,33 +3971,33 @@
       <c r="I7" s="1"/>
       <c r="J7" s="2"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="5"/>
+      <c r="L7" s="2"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="2"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="2" t="s">
         <v>181</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="2" t="s">
         <v>181</v>
       </c>
       <c r="G8" s="1"/>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="2" t="s">
         <v>181</v>
       </c>
       <c r="I8" s="1"/>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="2" t="s">
         <v>181</v>
       </c>
       <c r="K8" s="1"/>
-      <c r="L8" s="5"/>
+      <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="1" t="s">
@@ -4037,65 +4027,65 @@
         <v>181</v>
       </c>
       <c r="K9" s="1"/>
-      <c r="L9" s="5"/>
+      <c r="L9" s="2"/>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" s="2"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="2" t="s">
         <v>181</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="2"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="5"/>
+      <c r="H10" s="2"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="2" t="s">
         <v>181</v>
       </c>
       <c r="K10" s="1"/>
-      <c r="L10" s="5"/>
+      <c r="L10" s="2"/>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="2"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="5"/>
+      <c r="D11" s="2"/>
       <c r="E11" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="F11" s="6"/>
+      <c r="F11" s="2"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="5"/>
+      <c r="H11" s="2"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="5"/>
+      <c r="J11" s="2"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="5"/>
+      <c r="L11" s="2"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B12" s="2"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="5"/>
+      <c r="D12" s="2"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="5"/>
+      <c r="F12" s="2"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="5"/>
+      <c r="H12" s="2"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="5"/>
+      <c r="J12" s="2"/>
       <c r="K12" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="L12" s="2" t="s">
         <v>181</v>
       </c>
     </row>
@@ -4103,21 +4093,21 @@
       <c r="A13" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B13" s="5"/>
+      <c r="B13" s="2"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="5"/>
+      <c r="D13" s="2"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="5"/>
+      <c r="F13" s="2"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="2" t="s">
         <v>181</v>
       </c>
       <c r="I13" s="1"/>
-      <c r="J13" s="5"/>
+      <c r="J13" s="2"/>
       <c r="K13" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="L13" s="2" t="s">
         <v>181</v>
       </c>
     </row>
@@ -4125,21 +4115,21 @@
       <c r="A14" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B14" s="5"/>
+      <c r="B14" s="2"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="5"/>
+      <c r="D14" s="2"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="5"/>
+      <c r="F14" s="2"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="2" t="s">
         <v>181</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="5"/>
+      <c r="J14" s="2"/>
       <c r="K14" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="L14" s="2" t="s">
         <v>181</v>
       </c>
     </row>
@@ -4147,61 +4137,45 @@
       <c r="A15" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B15" s="5"/>
+      <c r="B15" s="2"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="5"/>
+      <c r="D15" s="2"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="5"/>
+      <c r="F15" s="2"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="5"/>
+      <c r="H15" s="2"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="5" t="s">
+      <c r="J15" s="2" t="s">
         <v>181</v>
       </c>
       <c r="K15" s="1"/>
-      <c r="L15" s="5"/>
+      <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B16" s="5"/>
+      <c r="B16" s="2"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="5"/>
+      <c r="D16" s="2"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="5"/>
+      <c r="F16" s="2"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="5" t="s">
+      <c r="H16" s="2" t="s">
         <v>181</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="J16" s="5"/>
+      <c r="J16" s="2"/>
       <c r="K16" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="L16" s="5"/>
+      <c r="L16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
-  <sheetData/>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
-</worksheet>
 </file>
</xml_diff>